<commit_message>
Tested with Standardization and kNN Imputer
</commit_message>
<xml_diff>
--- a/CaseStudy/Export/Correlation.xlsx
+++ b/CaseStudy/Export/Correlation.xlsx
@@ -593,82 +593,82 @@
         <v>-0.007008472659042641</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.005070223811740539</v>
+        <v>-0.005070223811738058</v>
       </c>
       <c r="E2" t="n">
-        <v>0.007199714812955415</v>
+        <v>0.007199714812957908</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0007085235742570927</v>
+        <v>-0.0007085235742506061</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001996650017355892</v>
+        <v>0.001996650017357398</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.01344581076908236</v>
+        <v>-0.01344581076908015</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00532784394233237</v>
+        <v>0.005327843942331428</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.006751821148455133</v>
+        <v>-0.006751821148425145</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.004841507045589921</v>
+        <v>-0.004841507045589334</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.003810115400934376</v>
+        <v>-0.003810115400934034</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.007806676320154362</v>
+        <v>-0.007806676320152247</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.001954009510647754</v>
+        <v>-0.001954009510615686</v>
       </c>
       <c r="O2" t="n">
-        <v>0.005819122517400565</v>
+        <v>0.005819122517392793</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.008440869839974836</v>
+        <v>-0.008440869839978979</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.01582495487227504</v>
+        <v>-0.01582495487227976</v>
       </c>
       <c r="R2" t="n">
-        <v>0.002415649425689221</v>
+        <v>0.002415649425692551</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.0009807823932810578</v>
+        <v>-0.0009807823932814451</v>
       </c>
       <c r="T2" t="n">
-        <v>0.003911157232875833</v>
+        <v>0.003911157232878403</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0005967040528196768</v>
+        <v>0.0005967040528228183</v>
       </c>
       <c r="V2" t="n">
-        <v>0.009497326623880441</v>
+        <v>0.009497326623859647</v>
       </c>
       <c r="W2" t="n">
-        <v>0.002941432585387207</v>
+        <v>0.00294143258538511</v>
       </c>
       <c r="X2" t="n">
-        <v>0.005003910971445519</v>
+        <v>0.005003910971446085</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0008010430298418943</v>
+        <v>0.0008010430298134766</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.009408097150033124</v>
+        <v>-0.009408097150011193</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.005426099532319422</v>
+        <v>0.005426099532313172</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.004392818585108896</v>
+        <v>-0.004392818585115982</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.01082710065890249</v>
+        <v>-0.01082710065890333</v>
       </c>
       <c r="AD2" t="n">
         <v>-0.007993536627121576</v>
@@ -687,82 +687,82 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05044208461916718</v>
+        <v>0.05044208461916696</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06779927667854051</v>
+        <v>0.06779927667853999</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.04645467609019956</v>
+        <v>-0.04645467609019886</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.01877136399188548</v>
+        <v>-0.01877136399188564</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1347852553956616</v>
+        <v>0.1347852553956619</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.05595703662236389</v>
+        <v>-0.05595703662236306</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0670079299603261</v>
+        <v>-0.06700792996032565</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.02412574075441356</v>
+        <v>-0.02412574075441339</v>
       </c>
       <c r="L3" t="n">
-        <v>0.05671463919688067</v>
+        <v>0.0567146391968809</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.02621911321679691</v>
+        <v>-0.02621911321679688</v>
       </c>
       <c r="N3" t="n">
-        <v>0.02516347794757309</v>
+        <v>0.02516347794757303</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.002006199593661594</v>
+        <v>-0.002006199593661507</v>
       </c>
       <c r="P3" t="n">
-        <v>0.04407645986771017</v>
+        <v>0.04407645986771008</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.118973569968957</v>
+        <v>0.1189735699689563</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.04221801463848562</v>
+        <v>-0.04221801463848525</v>
       </c>
       <c r="S3" t="n">
-        <v>0.07034325736537446</v>
+        <v>0.0703432573653735</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.003794108679387372</v>
+        <v>-0.003794108679387379</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.04578648021525906</v>
+        <v>-0.0457864802152591</v>
       </c>
       <c r="V3" t="n">
-        <v>0.02781125497952122</v>
+        <v>0.02781125497952166</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04481943691241007</v>
+        <v>0.04481943691241014</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.0358605225742939</v>
+        <v>-0.03586052257429424</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.0125200163497233</v>
+        <v>0.01252001634972355</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.003483363700039387</v>
+        <v>-0.003483363700040023</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.0661294438138972</v>
+        <v>-0.06612944381389659</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.01355440587483009</v>
+        <v>0.01355440587483</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.0842009076313234</v>
+        <v>0.084200907631323</v>
       </c>
       <c r="AD3" t="n">
         <v>0.0106089585031679</v>
@@ -775,91 +775,91 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.005070223811740539</v>
+        <v>-0.005070223811738058</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05044208461916718</v>
+        <v>0.05044208461916696</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2854228459919279</v>
+        <v>-0.2854228459919291</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03876588119624878</v>
+        <v>0.03876588119624808</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1031036205733099</v>
+        <v>0.1031036205733086</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0250676840370101</v>
+        <v>0.02506768403700984</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.1240683217221162</v>
+        <v>-0.1240683217221154</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2015400208497252</v>
+        <v>0.2015400208497256</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2244892493389928</v>
+        <v>0.2244892493389906</v>
       </c>
       <c r="L4" t="n">
-        <v>0.127729567213234</v>
+        <v>0.1277295672132354</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2335739591475389</v>
+        <v>0.2335739591475398</v>
       </c>
       <c r="N4" t="n">
-        <v>0.04104506306654963</v>
+        <v>0.04104506306654939</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.1093791755856602</v>
+        <v>-0.1093791755856592</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2134837274346923</v>
+        <v>0.2134837274346892</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1232799394662013</v>
+        <v>0.1232799394661991</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.2211626770849119</v>
+        <v>-0.2211626770849093</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.1342813671830736</v>
+        <v>-0.1342813671830702</v>
       </c>
       <c r="T4" t="n">
-        <v>0.03189711144304417</v>
+        <v>0.03189711144304377</v>
       </c>
       <c r="U4" t="n">
-        <v>0.05370476839399517</v>
+        <v>0.05370476839399391</v>
       </c>
       <c r="V4" t="n">
-        <v>0.03663948474760154</v>
+        <v>0.03663948474760128</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.108249922874552</v>
+        <v>-0.1082499228745516</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.06455220261611155</v>
+        <v>-0.06455220261611073</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.08380594414087883</v>
+        <v>0.08380594414087869</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2568660344935288</v>
+        <v>0.2568660344935301</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.02677572435974179</v>
+        <v>-0.02677572435974134</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.04137257711003997</v>
+        <v>0.04137257711004026</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.01170716638941764</v>
+        <v>0.01170716638941757</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.004544723741324455</v>
+        <v>0.00454472374132441</v>
       </c>
     </row>
     <row r="5">
@@ -869,91 +869,91 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.007199714812955415</v>
+        <v>0.007199714812957908</v>
       </c>
       <c r="C5" t="n">
-        <v>0.06779927667854051</v>
+        <v>0.06779927667853999</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2854228459919279</v>
+        <v>-0.2854228459919291</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1659442236438834</v>
+        <v>-0.1659442236438829</v>
       </c>
       <c r="G5" t="n">
         <v>-0.1915984574506099</v>
       </c>
       <c r="H5" t="n">
-        <v>0.03178008536421172</v>
+        <v>0.03178008536421191</v>
       </c>
       <c r="I5" t="n">
-        <v>0.133243164118091</v>
+        <v>0.1332431641180928</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.1588929993566435</v>
+        <v>-0.1588929993566444</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1359016179997423</v>
+        <v>-0.1359016179997409</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.09482163926037128</v>
+        <v>-0.09482163926037218</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1841377598445458</v>
+        <v>-0.1841377598445468</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.01823123135068536</v>
+        <v>-0.01823123135068524</v>
       </c>
       <c r="O5" t="n">
-        <v>0.06488022195694126</v>
+        <v>0.06488022195694104</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1610312267027526</v>
+        <v>-0.1610312267027513</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.06471908231036332</v>
+        <v>-0.06471908231036244</v>
       </c>
       <c r="R5" t="n">
-        <v>0.2137294667945394</v>
+        <v>0.2137294667945424</v>
       </c>
       <c r="S5" t="n">
-        <v>0.2404141307388282</v>
+        <v>0.2404141307388312</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.08699327581894833</v>
+        <v>-0.08699327581894981</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.1647399506653904</v>
+        <v>-0.1647399506653912</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.009927045468401442</v>
+        <v>-0.009927045468401587</v>
       </c>
       <c r="W5" t="n">
-        <v>0.1857402266390834</v>
+        <v>0.1857402266390846</v>
       </c>
       <c r="X5" t="n">
-        <v>0.01048213081496958</v>
+        <v>0.0104821308149696</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.06123995584416253</v>
+        <v>-0.06123995584416318</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.1421976854004575</v>
+        <v>-0.1421976854004574</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.050870085872</v>
+        <v>-0.05087008587199935</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.07113979528195961</v>
+        <v>-0.07113979528195999</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.08153572737599171</v>
+        <v>0.0815357273759923</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.009027057405997655</v>
+        <v>-0.009027057405997772</v>
       </c>
     </row>
     <row r="6">
@@ -963,91 +963,91 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0007085235742570927</v>
+        <v>-0.0007085235742506061</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.04645467609019956</v>
+        <v>-0.04645467609019886</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03876588119624878</v>
+        <v>0.03876588119624808</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1659442236438834</v>
+        <v>-0.1659442236438829</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3937092311458022</v>
+        <v>0.3937092311458016</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1647710451171673</v>
+        <v>-0.1647710451171668</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06749129753345906</v>
+        <v>0.06749129753345921</v>
       </c>
       <c r="J6" t="n">
-        <v>0.08677317706123716</v>
+        <v>0.0867731770612358</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.08367488681719205</v>
+        <v>-0.08367488681719192</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.06399826795457395</v>
+        <v>-0.06399826795457438</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0669541206619178</v>
+        <v>0.06695412066191682</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0910335862665632</v>
+        <v>-0.0910335862665629</v>
       </c>
       <c r="O6" t="n">
-        <v>0.00817052050051081</v>
+        <v>0.00817052050051075</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0613281505858559</v>
+        <v>-0.06132815058585541</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.142484839532165</v>
+        <v>-0.1424848395321638</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0536351020726376</v>
+        <v>0.05363510207263694</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.1108649630770487</v>
+        <v>-0.1108649630770478</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.005657214339024793</v>
+        <v>-0.005657214339024754</v>
       </c>
       <c r="U6" t="n">
-        <v>0.516338991603269</v>
+        <v>0.5163389916032641</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1089322791113146</v>
+        <v>-0.1089322791113128</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.09901520957341113</v>
+        <v>-0.09901520957340881</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0735867004219814</v>
+        <v>0.07358670042198172</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.04788222386583905</v>
+        <v>-0.04788222386583824</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.1206321809120469</v>
+        <v>-0.1206321809120477</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1230084554100962</v>
+        <v>0.1230084554100948</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.03274846807870283</v>
+        <v>-0.03274846807870237</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.1495979406489653</v>
+        <v>-0.1495979406489637</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.001918246918019292</v>
+        <v>0.001918246918019185</v>
       </c>
     </row>
     <row r="7">
@@ -1057,91 +1057,91 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001996650017355892</v>
+        <v>0.001996650017357398</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.01877136399188548</v>
+        <v>-0.01877136399188564</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1031036205733099</v>
+        <v>0.1031036205733086</v>
       </c>
       <c r="E7" t="n">
         <v>-0.1915984574506099</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3937092311458022</v>
+        <v>0.3937092311458016</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.01744445223407568</v>
+        <v>-0.01744445223407567</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.01110522927200638</v>
+        <v>-0.01110522927200634</v>
       </c>
       <c r="J7" t="n">
-        <v>0.09359933008622717</v>
+        <v>0.09359933008622667</v>
       </c>
       <c r="K7" t="n">
-        <v>0.04884581038940236</v>
+        <v>0.04884581038940265</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.06480089222744057</v>
+        <v>-0.06480089222744193</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2183685993399895</v>
+        <v>0.2183685993399871</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.01106716854842715</v>
+        <v>-0.0110671685484269</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.06144647528048693</v>
+        <v>-0.061446475280487</v>
       </c>
       <c r="P7" t="n">
-        <v>0.05745204772809327</v>
+        <v>0.05745204772809384</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.1017707294568496</v>
+        <v>-0.1017707294568489</v>
       </c>
       <c r="R7" t="n">
-        <v>0.08547959274002565</v>
+        <v>0.08547959274002555</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.1396715866169315</v>
+        <v>-0.1396715866169304</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1474424934269183</v>
+        <v>0.1474424934269196</v>
       </c>
       <c r="U7" t="n">
-        <v>0.3769693384788033</v>
+        <v>0.376969338478802</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.03178511420970341</v>
+        <v>-0.0317851142097036</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.09664702363980325</v>
+        <v>-0.09664702363980367</v>
       </c>
       <c r="X7" t="n">
-        <v>0.04811196699130712</v>
+        <v>0.0481119669913073</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.01688105226224058</v>
+        <v>0.0168810522622406</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.05101035330868532</v>
+        <v>-0.05101035330868514</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.09573980675138695</v>
+        <v>0.09573980675138585</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.0109430165515314</v>
+        <v>0.01094301655153136</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.1613721687741418</v>
+        <v>-0.161372168774144</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.0004213666633361417</v>
+        <v>0.000421366663336117</v>
       </c>
     </row>
     <row r="8">
@@ -1151,91 +1151,91 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.01344581076908236</v>
+        <v>-0.01344581076908015</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1347852553956616</v>
+        <v>0.1347852553956619</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0250676840370101</v>
+        <v>0.02506768403700984</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03178008536421172</v>
+        <v>0.03178008536421191</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1647710451171673</v>
+        <v>-0.1647710451171668</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01744445223407568</v>
+        <v>-0.01744445223407567</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.1025703582654419</v>
+        <v>-0.1025703582654423</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.08882547027173551</v>
+        <v>-0.08882547027173492</v>
       </c>
       <c r="K8" t="n">
-        <v>0.03967748778025353</v>
+        <v>0.03967748778025364</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1433809049780108</v>
+        <v>0.143380904978012</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01006404030103051</v>
+        <v>0.01006404030103045</v>
       </c>
       <c r="N8" t="n">
-        <v>0.06650253986622781</v>
+        <v>0.06650253986622809</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.08329810050424606</v>
+        <v>-0.08329810050424556</v>
       </c>
       <c r="P8" t="n">
-        <v>0.08274365449228943</v>
+        <v>0.08274365449228922</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2116712719142603</v>
+        <v>0.2116712719142572</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1602828742365804</v>
+        <v>-0.1602828742365812</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04686897793799323</v>
+        <v>0.04686897793799374</v>
       </c>
       <c r="T8" t="n">
         <v>-0.1027593134180955</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.1563366399626702</v>
+        <v>-0.1563366399626703</v>
       </c>
       <c r="V8" t="n">
-        <v>0.08150582366447642</v>
+        <v>0.08150582366447644</v>
       </c>
       <c r="W8" t="n">
-        <v>0.02306022491483493</v>
+        <v>0.02306022491483497</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.07774297094939014</v>
+        <v>-0.07774297094939057</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.06837757927492207</v>
+        <v>0.06837757927492243</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.06111048046672673</v>
+        <v>0.06111048046672687</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.2779357062449836</v>
+        <v>-0.2779357062449813</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.04252764104902889</v>
+        <v>-0.0425276410490285</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1849532431283435</v>
+        <v>0.1849532431283424</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.005426109759395114</v>
+        <v>0.005426109759395126</v>
       </c>
     </row>
     <row r="9">
@@ -1245,91 +1245,91 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.00532784394233237</v>
+        <v>0.005327843942331428</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.05595703662236389</v>
+        <v>-0.05595703662236306</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1240683217221162</v>
+        <v>-0.1240683217221154</v>
       </c>
       <c r="E9" t="n">
-        <v>0.133243164118091</v>
+        <v>0.1332431641180928</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06749129753345906</v>
+        <v>0.06749129753345921</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01110522927200638</v>
+        <v>-0.01110522927200634</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1025703582654419</v>
+        <v>-0.1025703582654423</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.04955528768131017</v>
+        <v>-0.04955528768131071</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.05948150968660529</v>
+        <v>-0.05948150968660513</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.08493555240859314</v>
+        <v>-0.08493555240859298</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.04870524949385754</v>
+        <v>-0.04870524949385737</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01672970707055845</v>
+        <v>0.01672970707055853</v>
       </c>
       <c r="O9" t="n">
-        <v>0.03734049381615783</v>
+        <v>0.03734049381615734</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.1528584043154058</v>
+        <v>-0.1528584043154071</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.2386848625694477</v>
+        <v>-0.238684862569447</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1362566916341267</v>
+        <v>0.1362566916341287</v>
       </c>
       <c r="S9" t="n">
-        <v>0.04036997884390937</v>
+        <v>0.04036997884390919</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.09518456050552647</v>
+        <v>-0.09518456050552666</v>
       </c>
       <c r="U9" t="n">
-        <v>0.04955333063480253</v>
+        <v>0.04955333063480254</v>
       </c>
       <c r="V9" t="n">
-        <v>0.03914221414788874</v>
+        <v>0.0391422141478881</v>
       </c>
       <c r="W9" t="n">
-        <v>0.05948459823898868</v>
+        <v>0.05948459823898915</v>
       </c>
       <c r="X9" t="n">
-        <v>0.2163664193155172</v>
+        <v>0.2163664193155169</v>
       </c>
       <c r="Y9" t="n">
-        <v>-0.001998790661104619</v>
+        <v>-0.001998790661104742</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.08980249677434633</v>
+        <v>-0.08980249677434596</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.01072743307583247</v>
+        <v>0.01072743307583234</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.1566592073495101</v>
+        <v>-0.1566592073495103</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.02058144507498665</v>
+        <v>-0.02058144507498651</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.007568510999958534</v>
+        <v>-0.007568510999958596</v>
       </c>
     </row>
     <row r="10">
@@ -1339,91 +1339,91 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.006751821148455133</v>
+        <v>-0.006751821148425145</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0670079299603261</v>
+        <v>-0.06700792996032565</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2015400208497252</v>
+        <v>0.2015400208497256</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1588929993566435</v>
+        <v>-0.1588929993566444</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08677317706123716</v>
+        <v>0.0867731770612358</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09359933008622717</v>
+        <v>0.09359933008622667</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.08882547027173551</v>
+        <v>-0.08882547027173492</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.04955528768131017</v>
+        <v>-0.04955528768131071</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.3845128053578957</v>
+        <v>0.3845128053578986</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.01851781681925864</v>
+        <v>-0.01851781681925876</v>
       </c>
       <c r="M10" t="n">
-        <v>0.3670388156609249</v>
+        <v>0.3670388156609222</v>
       </c>
       <c r="N10" t="n">
-        <v>0.005383167161179466</v>
+        <v>0.005383167161180205</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.2719323436647441</v>
+        <v>-0.2719323436647439</v>
       </c>
       <c r="P10" t="n">
-        <v>0.09033857841294433</v>
+        <v>0.0903385784129466</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0002792881348068071</v>
+        <v>-0.0002792881348067672</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.04049457658265278</v>
+        <v>-0.04049457658265238</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.1919958065818631</v>
+        <v>-0.191995806581865</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.05152459165661784</v>
+        <v>-0.05152459165661902</v>
       </c>
       <c r="U10" t="n">
-        <v>0.09624459835032532</v>
+        <v>0.09624459835032548</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.01492358163074485</v>
+        <v>-0.01492358163074341</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.1715391509211246</v>
+        <v>-0.1715391509211264</v>
       </c>
       <c r="X10" t="n">
-        <v>0.004669191514804919</v>
+        <v>0.004669191514805735</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.04132731441204203</v>
+        <v>0.04132731441204204</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.418628273139914</v>
+        <v>0.418628273139917</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.03807358625458564</v>
+        <v>0.03807358625458487</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.02671046812049865</v>
+        <v>-0.02671046812049771</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.0283806244469918</v>
+        <v>-0.02838062444699174</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.008696629340338607</v>
+        <v>-0.008696629340339374</v>
       </c>
     </row>
     <row r="11">
@@ -1433,31 +1433,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.004841507045589921</v>
+        <v>-0.004841507045589334</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.02412574075441356</v>
+        <v>-0.02412574075441339</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2244892493389928</v>
+        <v>0.2244892493389906</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1359016179997423</v>
+        <v>-0.1359016179997409</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.08367488681719205</v>
+        <v>-0.08367488681719192</v>
       </c>
       <c r="G11" t="n">
-        <v>0.04884581038940236</v>
+        <v>0.04884581038940265</v>
       </c>
       <c r="H11" t="n">
-        <v>0.03967748778025353</v>
+        <v>0.03967748778025364</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.05948150968660529</v>
+        <v>-0.05948150968660513</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3845128053578957</v>
+        <v>0.3845128053578986</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
@@ -1466,58 +1466,58 @@
         <v>0.05342650259919801</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4110876095477542</v>
+        <v>0.4110876095477534</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0819177116426527</v>
+        <v>0.08191771164265173</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.2023785527404743</v>
+        <v>-0.2023785527404742</v>
       </c>
       <c r="P11" t="n">
-        <v>0.174290094998102</v>
+        <v>0.1742900949981042</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.01807801528670424</v>
+        <v>0.01807801528670422</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.07889893462779807</v>
+        <v>-0.0788989346277989</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.1685112394032622</v>
+        <v>-0.1685112394032636</v>
       </c>
       <c r="T11" t="n">
-        <v>0.03973043369083385</v>
+        <v>0.03973043369083457</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.06432922574812154</v>
+        <v>-0.06432922574812137</v>
       </c>
       <c r="V11" t="n">
-        <v>0.07419310337784693</v>
+        <v>0.07419310337784719</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.1234197914188628</v>
+        <v>-0.123419791418862</v>
       </c>
       <c r="X11" t="n">
-        <v>0.01160106055080734</v>
+        <v>0.01160106055080736</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.08432036723016692</v>
+        <v>0.0843203672301677</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.4193997560018932</v>
+        <v>0.4193997560018921</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.0180122360040814</v>
+        <v>-0.01801223600408141</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.01440263580629536</v>
+        <v>0.01440263580629541</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.01724922605509063</v>
+        <v>-0.01724922605509062</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.004571282443345222</v>
+        <v>-0.004571282443345205</v>
       </c>
     </row>
     <row r="12">
@@ -1527,31 +1527,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.003810115400934376</v>
+        <v>-0.003810115400934034</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05671463919688067</v>
+        <v>0.0567146391968809</v>
       </c>
       <c r="D12" t="n">
-        <v>0.127729567213234</v>
+        <v>0.1277295672132354</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.09482163926037128</v>
+        <v>-0.09482163926037218</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.06399826795457395</v>
+        <v>-0.06399826795457438</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.06480089222744057</v>
+        <v>-0.06480089222744193</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1433809049780108</v>
+        <v>0.143380904978012</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.08493555240859314</v>
+        <v>-0.08493555240859298</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.01851781681925864</v>
+        <v>-0.01851781681925876</v>
       </c>
       <c r="K12" t="n">
         <v>0.05342650259919801</v>
@@ -1560,58 +1560,58 @@
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.02047199712390748</v>
+        <v>0.02047199712390744</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0483085480123429</v>
+        <v>0.04830854801234277</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.04625105774419681</v>
+        <v>-0.04625105774419682</v>
       </c>
       <c r="P12" t="n">
-        <v>0.3389168996468343</v>
+        <v>0.3389168996468365</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.1592280812505129</v>
+        <v>0.1592280812505132</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.324243374336253</v>
+        <v>-0.3242433743362566</v>
       </c>
       <c r="S12" t="n">
-        <v>0.02384017132183621</v>
+        <v>0.02384017132183658</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.06803133607450808</v>
+        <v>-0.06803133607450866</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.05220627135387298</v>
+        <v>-0.05220627135387299</v>
       </c>
       <c r="V12" t="n">
-        <v>0.05862524183523384</v>
+        <v>0.05862524183523415</v>
       </c>
       <c r="W12" t="n">
-        <v>0.03897303022562307</v>
+        <v>0.03897303022562335</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.07304035230077455</v>
+        <v>-0.07304035230077466</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.05257813613734239</v>
+        <v>0.05257813613734297</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.09762831260398865</v>
+        <v>0.09762831260398891</v>
       </c>
       <c r="AA12" t="n">
-        <v>-0.1584801244511929</v>
+        <v>-0.1584801244511936</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.04897913315473101</v>
+        <v>0.04897913315473058</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1466866568400325</v>
+        <v>0.1466866568400333</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.005873925907306311</v>
+        <v>0.005873925907306308</v>
       </c>
     </row>
     <row r="13">
@@ -1621,91 +1621,91 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.007806676320154362</v>
+        <v>-0.007806676320152247</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.02621911321679691</v>
+        <v>-0.02621911321679688</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2335739591475389</v>
+        <v>0.2335739591475398</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1841377598445458</v>
+        <v>-0.1841377598445468</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0669541206619178</v>
+        <v>0.06695412066191682</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2183685993399895</v>
+        <v>0.2183685993399871</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01006404030103051</v>
+        <v>0.01006404030103045</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.04870524949385754</v>
+        <v>-0.04870524949385737</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3670388156609249</v>
+        <v>0.3670388156609222</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4110876095477542</v>
+        <v>0.4110876095477534</v>
       </c>
       <c r="L13" t="n">
-        <v>0.02047199712390748</v>
+        <v>0.02047199712390744</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.04660949562149549</v>
+        <v>0.04660949562149439</v>
       </c>
       <c r="O13" t="n">
         <v>-0.1829286058876974</v>
       </c>
       <c r="P13" t="n">
-        <v>0.1668272179865355</v>
+        <v>0.1668272179865329</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.03234129421564737</v>
+        <v>-0.03234129421564733</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.03789591040141408</v>
+        <v>-0.03789591040141446</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.1734339124309828</v>
+        <v>-0.1734339124309823</v>
       </c>
       <c r="T13" t="n">
-        <v>0.09917256699636987</v>
+        <v>0.09917256699637013</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0760657367823839</v>
+        <v>0.07606573678238433</v>
       </c>
       <c r="V13" t="n">
-        <v>0.03624412638198279</v>
+        <v>0.03624412638198244</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.1375542232090765</v>
+        <v>-0.1375542232090763</v>
       </c>
       <c r="X13" t="n">
-        <v>0.01943064813602756</v>
+        <v>0.01943064813602745</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.06490096721177657</v>
+        <v>0.06490096721177659</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.2946619357661486</v>
+        <v>0.294661935766147</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.04040243838788284</v>
+        <v>0.04040243838788274</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.02113975537609423</v>
+        <v>0.02113975537609375</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.08553931658610751</v>
+        <v>-0.08553931658610614</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.01594584507032234</v>
+        <v>-0.01594584507032239</v>
       </c>
     </row>
     <row r="14">
@@ -1715,91 +1715,91 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001954009510647754</v>
+        <v>-0.001954009510615686</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02516347794757309</v>
+        <v>0.02516347794757303</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04104506306654963</v>
+        <v>0.04104506306654939</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01823123135068536</v>
+        <v>-0.01823123135068524</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0910335862665632</v>
+        <v>-0.0910335862665629</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.01106716854842715</v>
+        <v>-0.0110671685484269</v>
       </c>
       <c r="H14" t="n">
-        <v>0.06650253986622781</v>
+        <v>0.06650253986622809</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01672970707055845</v>
+        <v>0.01672970707055853</v>
       </c>
       <c r="J14" t="n">
-        <v>0.005383167161179466</v>
+        <v>0.005383167161180205</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0819177116426527</v>
+        <v>0.08191771164265173</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0483085480123429</v>
+        <v>0.04830854801234277</v>
       </c>
       <c r="M14" t="n">
-        <v>0.04660949562149549</v>
+        <v>0.04660949562149439</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.02952856641754138</v>
+        <v>-0.02952856641754083</v>
       </c>
       <c r="P14" t="n">
-        <v>0.07559323031462536</v>
+        <v>0.07559323031462437</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.001959905721662743</v>
+        <v>-0.001959905721663105</v>
       </c>
       <c r="R14" t="n">
         <v>-0.02891601454621705</v>
       </c>
       <c r="S14" t="n">
-        <v>0.004138345620604079</v>
+        <v>0.00413834562060411</v>
       </c>
       <c r="T14" t="n">
-        <v>0.002471891210657182</v>
+        <v>0.002471891210656967</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.08360957169362965</v>
+        <v>-0.08360957169362936</v>
       </c>
       <c r="V14" t="n">
-        <v>0.2769890893549909</v>
+        <v>0.2769890893549882</v>
       </c>
       <c r="W14" t="n">
-        <v>0.005493622971748061</v>
+        <v>0.005493622971748255</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0282435271655872</v>
+        <v>0.02824352716558755</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.3171485346167666</v>
+        <v>0.3171485346167626</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.03975230575459605</v>
+        <v>0.03975230575459551</v>
       </c>
       <c r="AA14" t="n">
-        <v>-0.03988356159728796</v>
+        <v>-0.03988356159728736</v>
       </c>
       <c r="AB14" t="n">
-        <v>-0.01023285931755934</v>
+        <v>-0.01023285931755932</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.01462849170605041</v>
+        <v>0.01462849170605009</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.004039404939309665</v>
+        <v>-0.00403940493930977</v>
       </c>
     </row>
     <row r="15">
@@ -1809,91 +1809,91 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.005819122517400565</v>
+        <v>0.005819122517392793</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.002006199593661594</v>
+        <v>-0.002006199593661507</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.1093791755856602</v>
+        <v>-0.1093791755856592</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06488022195694126</v>
+        <v>0.06488022195694104</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00817052050051081</v>
+        <v>0.00817052050051075</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.06144647528048693</v>
+        <v>-0.061446475280487</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.08329810050424606</v>
+        <v>-0.08329810050424556</v>
       </c>
       <c r="I15" t="n">
-        <v>0.03734049381615783</v>
+        <v>0.03734049381615734</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.2719323436647441</v>
+        <v>-0.2719323436647439</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.2023785527404743</v>
+        <v>-0.2023785527404742</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.04625105774419681</v>
+        <v>-0.04625105774419682</v>
       </c>
       <c r="M15" t="n">
         <v>-0.1829286058876974</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.02952856641754138</v>
+        <v>-0.02952856641754083</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.06678504073408892</v>
+        <v>-0.066785040734088</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0471293049239924</v>
+        <v>-0.0471293049239919</v>
       </c>
       <c r="R15" t="n">
-        <v>0.07524189848482278</v>
+        <v>0.07524189848482273</v>
       </c>
       <c r="S15" t="n">
-        <v>0.06628040311839155</v>
+        <v>0.06628040311839081</v>
       </c>
       <c r="T15" t="n">
-        <v>0.02197973365535782</v>
+        <v>0.02197973365535795</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.0120577283038844</v>
+        <v>-0.01205772830388437</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.05007367349742455</v>
+        <v>-0.0500736734974245</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.001486675404982053</v>
+        <v>-0.001486675404982047</v>
       </c>
       <c r="X15" t="n">
-        <v>0.02387392725260601</v>
+        <v>0.02387392725260604</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.02634277216924626</v>
+        <v>-0.02634277216924662</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.2733345542053867</v>
+        <v>-0.273334554205385</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.05745802077997252</v>
+        <v>0.05745802077997238</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.0006378176445430204</v>
+        <v>0.0006378176445429979</v>
       </c>
       <c r="AC15" t="n">
-        <v>-0.04060749642768548</v>
+        <v>-0.04060749642768538</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.004234008957905645</v>
+        <v>-0.004234008957905523</v>
       </c>
     </row>
     <row r="16">
@@ -1903,91 +1903,91 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.008440869839974836</v>
+        <v>-0.008440869839978979</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04407645986771017</v>
+        <v>0.04407645986771008</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2134837274346923</v>
+        <v>0.2134837274346892</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1610312267027526</v>
+        <v>-0.1610312267027513</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0613281505858559</v>
+        <v>-0.06132815058585541</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05745204772809327</v>
+        <v>0.05745204772809384</v>
       </c>
       <c r="H16" t="n">
-        <v>0.08274365449228943</v>
+        <v>0.08274365449228922</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.1528584043154058</v>
+        <v>-0.1528584043154071</v>
       </c>
       <c r="J16" t="n">
-        <v>0.09033857841294433</v>
+        <v>0.0903385784129466</v>
       </c>
       <c r="K16" t="n">
-        <v>0.174290094998102</v>
+        <v>0.1742900949981042</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3389168996468343</v>
+        <v>0.3389168996468365</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1668272179865355</v>
+        <v>0.1668272179865329</v>
       </c>
       <c r="N16" t="n">
-        <v>0.07559323031462536</v>
+        <v>0.07559323031462437</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.06678504073408892</v>
+        <v>-0.066785040734088</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1206655757628114</v>
+        <v>0.1206655757628095</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.2661341157651904</v>
+        <v>-0.2661341157651934</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.04765287573683512</v>
+        <v>-0.0476528757368349</v>
       </c>
       <c r="T16" t="n">
-        <v>0.07423366367766596</v>
+        <v>0.07423366367766554</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.05465711834592554</v>
+        <v>-0.0546571183459256</v>
       </c>
       <c r="V16" t="n">
-        <v>0.04578199743103132</v>
+        <v>0.04578199743103103</v>
       </c>
       <c r="W16" t="n">
-        <v>0.002483263557514506</v>
+        <v>0.002483263557514441</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.05720384552394039</v>
+        <v>-0.05720384552394082</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.07505107035809126</v>
+        <v>0.07505107035809171</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.1967676808498771</v>
+        <v>0.1967676808498794</v>
       </c>
       <c r="AA16" t="n">
-        <v>-0.02532082955913875</v>
+        <v>-0.02532082955913859</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.100842758956742</v>
+        <v>0.1008427589567406</v>
       </c>
       <c r="AC16" t="n">
-        <v>-0.005912817915373824</v>
+        <v>-0.005912817915373845</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.001272051356885027</v>
+        <v>0.001272051356885095</v>
       </c>
     </row>
     <row r="17">
@@ -1997,91 +1997,91 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01582495487227504</v>
+        <v>-0.01582495487227976</v>
       </c>
       <c r="C17" t="n">
-        <v>0.118973569968957</v>
+        <v>0.1189735699689563</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1232799394662013</v>
+        <v>0.1232799394661991</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.06471908231036332</v>
+        <v>-0.06471908231036244</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.142484839532165</v>
+        <v>-0.1424848395321638</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.1017707294568496</v>
+        <v>-0.1017707294568489</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2116712719142603</v>
+        <v>0.2116712719142572</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.2386848625694477</v>
+        <v>-0.238684862569447</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.0002792881348068071</v>
+        <v>-0.0002792881348067672</v>
       </c>
       <c r="K17" t="n">
-        <v>0.01807801528670424</v>
+        <v>0.01807801528670422</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1592280812505129</v>
+        <v>0.1592280812505132</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.03234129421564737</v>
+        <v>-0.03234129421564733</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.001959905721662743</v>
+        <v>-0.001959905721663105</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.0471293049239924</v>
+        <v>-0.0471293049239919</v>
       </c>
       <c r="P17" t="n">
-        <v>0.1206655757628114</v>
+        <v>0.1206655757628095</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.1885515900137799</v>
+        <v>-0.1885515900137784</v>
       </c>
       <c r="S17" t="n">
-        <v>0.04922211831063138</v>
+        <v>0.04922211831063129</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.1496110297052771</v>
+        <v>-0.1496110297052797</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.103698342794782</v>
+        <v>-0.1036983427947809</v>
       </c>
       <c r="V17" t="n">
-        <v>0.001158733198858472</v>
+        <v>0.001158733198858716</v>
       </c>
       <c r="W17" t="n">
-        <v>0.03767108432824334</v>
+        <v>0.03767108432824318</v>
       </c>
       <c r="X17" t="n">
-        <v>-0.1315965272369784</v>
+        <v>-0.1315965272369776</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.001188264917783325</v>
+        <v>0.001188264917783762</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.09736058552479951</v>
+        <v>0.09736058552480011</v>
       </c>
       <c r="AA17" t="n">
-        <v>-0.179934843894821</v>
+        <v>-0.1799348438948209</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.01928345916355061</v>
+        <v>0.01928345916355012</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.2774237764659984</v>
+        <v>0.2774237764659986</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.004219300638306392</v>
+        <v>0.004219300638306309</v>
       </c>
     </row>
     <row r="18">
@@ -2091,91 +2091,91 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002415649425689221</v>
+        <v>0.002415649425692551</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.04221801463848562</v>
+        <v>-0.04221801463848525</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.2211626770849119</v>
+        <v>-0.2211626770849093</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2137294667945394</v>
+        <v>0.2137294667945424</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0536351020726376</v>
+        <v>0.05363510207263694</v>
       </c>
       <c r="G18" t="n">
-        <v>0.08547959274002565</v>
+        <v>0.08547959274002555</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.1602828742365804</v>
+        <v>-0.1602828742365812</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1362566916341267</v>
+        <v>0.1362566916341287</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.04049457658265278</v>
+        <v>-0.04049457658265238</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.07889893462779807</v>
+        <v>-0.0788989346277989</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.324243374336253</v>
+        <v>-0.3242433743362566</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.03789591040141408</v>
+        <v>-0.03789591040141446</v>
       </c>
       <c r="N18" t="n">
         <v>-0.02891601454621705</v>
       </c>
       <c r="O18" t="n">
-        <v>0.07524189848482278</v>
+        <v>0.07524189848482273</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.2661341157651904</v>
+        <v>-0.2661341157651934</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.1885515900137799</v>
+        <v>-0.1885515900137784</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>0.02956655358049631</v>
+        <v>0.02956655358049609</v>
       </c>
       <c r="T18" t="n">
-        <v>0.1312233563446126</v>
+        <v>0.1312233563446141</v>
       </c>
       <c r="U18" t="n">
-        <v>0.03637625638365085</v>
+        <v>0.03637625638365086</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.04523204088140949</v>
+        <v>-0.04523204088140973</v>
       </c>
       <c r="W18" t="n">
-        <v>0.02985138372821214</v>
+        <v>0.02985138372821246</v>
       </c>
       <c r="X18" t="n">
-        <v>0.07424054917440119</v>
+        <v>0.07424054917440127</v>
       </c>
       <c r="Y18" t="n">
-        <v>-0.02442188641142188</v>
+        <v>-0.02442188641142184</v>
       </c>
       <c r="Z18" t="n">
-        <v>-0.1364583303218727</v>
+        <v>-0.1364583303218744</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1970722535658273</v>
+        <v>0.1970722535658275</v>
       </c>
       <c r="AB18" t="n">
-        <v>-0.01723209823915177</v>
+        <v>-0.01723209823915158</v>
       </c>
       <c r="AC18" t="n">
-        <v>-0.1640239568781148</v>
+        <v>-0.1640239568781167</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.004214917736628397</v>
+        <v>0.004214917736628346</v>
       </c>
     </row>
     <row r="19">
@@ -2185,91 +2185,91 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.0009807823932810578</v>
+        <v>-0.0009807823932814451</v>
       </c>
       <c r="C19" t="n">
-        <v>0.07034325736537446</v>
+        <v>0.0703432573653735</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.1342813671830736</v>
+        <v>-0.1342813671830702</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2404141307388282</v>
+        <v>0.2404141307388312</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.1108649630770487</v>
+        <v>-0.1108649630770478</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.1396715866169315</v>
+        <v>-0.1396715866169304</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04686897793799323</v>
+        <v>0.04686897793799374</v>
       </c>
       <c r="I19" t="n">
-        <v>0.04036997884390937</v>
+        <v>0.04036997884390919</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.1919958065818631</v>
+        <v>-0.191995806581865</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.1685112394032622</v>
+        <v>-0.1685112394032636</v>
       </c>
       <c r="L19" t="n">
-        <v>0.02384017132183621</v>
+        <v>0.02384017132183658</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.1734339124309828</v>
+        <v>-0.1734339124309823</v>
       </c>
       <c r="N19" t="n">
-        <v>0.004138345620604079</v>
+        <v>0.00413834562060411</v>
       </c>
       <c r="O19" t="n">
-        <v>0.06628040311839155</v>
+        <v>0.06628040311839081</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.04765287573683512</v>
+        <v>-0.0476528757368349</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.04922211831063138</v>
+        <v>0.04922211831063129</v>
       </c>
       <c r="R19" t="n">
-        <v>0.02956655358049631</v>
+        <v>0.02956655358049609</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.1162433577448628</v>
+        <v>-0.1162433577448635</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.1100962586465691</v>
+        <v>-0.1100962586465682</v>
       </c>
       <c r="V19" t="n">
-        <v>0.007222014700928866</v>
+        <v>0.007222014700928612</v>
       </c>
       <c r="W19" t="n">
-        <v>0.3806254518602876</v>
+        <v>0.3806254518602838</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.04302614111301012</v>
+        <v>-0.04302614111301006</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.03899381807571244</v>
+        <v>-0.03899381807571276</v>
       </c>
       <c r="Z19" t="n">
-        <v>-0.190701823841399</v>
+        <v>-0.1907018238413989</v>
       </c>
       <c r="AA19" t="n">
-        <v>-0.07509590136447311</v>
+        <v>-0.07509590136447344</v>
       </c>
       <c r="AB19" t="n">
-        <v>-0.04155875220409582</v>
+        <v>-0.04155875220409568</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1281674556597141</v>
+        <v>0.1281674556597133</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.005855144767080881</v>
+        <v>0.005855144767080836</v>
       </c>
     </row>
     <row r="20">
@@ -2279,91 +2279,91 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003911157232875833</v>
+        <v>0.003911157232878403</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.003794108679387372</v>
+        <v>-0.003794108679387379</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03189711144304417</v>
+        <v>0.03189711144304377</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.08699327581894833</v>
+        <v>-0.08699327581894981</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.005657214339024793</v>
+        <v>-0.005657214339024754</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1474424934269183</v>
+        <v>0.1474424934269196</v>
       </c>
       <c r="H20" t="n">
         <v>-0.1027593134180955</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.09518456050552647</v>
+        <v>-0.09518456050552666</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.05152459165661784</v>
+        <v>-0.05152459165661902</v>
       </c>
       <c r="K20" t="n">
-        <v>0.03973043369083385</v>
+        <v>0.03973043369083457</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.06803133607450808</v>
+        <v>-0.06803133607450866</v>
       </c>
       <c r="M20" t="n">
-        <v>0.09917256699636987</v>
+        <v>0.09917256699637013</v>
       </c>
       <c r="N20" t="n">
-        <v>0.002471891210657182</v>
+        <v>0.002471891210656967</v>
       </c>
       <c r="O20" t="n">
-        <v>0.02197973365535782</v>
+        <v>0.02197973365535795</v>
       </c>
       <c r="P20" t="n">
-        <v>0.07423366367766596</v>
+        <v>0.07423366367766554</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.1496110297052771</v>
+        <v>-0.1496110297052797</v>
       </c>
       <c r="R20" t="n">
-        <v>0.1312233563446126</v>
+        <v>0.1312233563446141</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.1162433577448628</v>
+        <v>-0.1162433577448635</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
       </c>
       <c r="U20" t="n">
-        <v>-0.006222482790362939</v>
+        <v>-0.006222482790362905</v>
       </c>
       <c r="V20" t="n">
         <v>-0.01596469403155534</v>
       </c>
       <c r="W20" t="n">
-        <v>-0.1145480770662133</v>
+        <v>-0.1145480770662147</v>
       </c>
       <c r="X20" t="n">
-        <v>0.04166142694064974</v>
+        <v>0.04166142694064977</v>
       </c>
       <c r="Y20" t="n">
-        <v>-0.007910229573284319</v>
+        <v>-0.00791022957328465</v>
       </c>
       <c r="Z20" t="n">
-        <v>-0.04008735733789851</v>
+        <v>-0.04008735733789861</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.2649765140623815</v>
+        <v>0.2649765140623843</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.3991755876204435</v>
+        <v>0.399175587620446</v>
       </c>
       <c r="AC20" t="n">
-        <v>-0.2752613552520654</v>
+        <v>-0.2752613552520646</v>
       </c>
       <c r="AD20" t="n">
-        <v>-0.0003191464164218632</v>
+        <v>-0.0003191464164218972</v>
       </c>
     </row>
     <row r="21">
@@ -2373,91 +2373,91 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0005967040528196768</v>
+        <v>0.0005967040528228183</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.04578648021525906</v>
+        <v>-0.0457864802152591</v>
       </c>
       <c r="D21" t="n">
-        <v>0.05370476839399517</v>
+        <v>0.05370476839399391</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.1647399506653904</v>
+        <v>-0.1647399506653912</v>
       </c>
       <c r="F21" t="n">
-        <v>0.516338991603269</v>
+        <v>0.5163389916032641</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3769693384788033</v>
+        <v>0.376969338478802</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.1563366399626702</v>
+        <v>-0.1563366399626703</v>
       </c>
       <c r="I21" t="n">
-        <v>0.04955333063480253</v>
+        <v>0.04955333063480254</v>
       </c>
       <c r="J21" t="n">
-        <v>0.09624459835032532</v>
+        <v>0.09624459835032548</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.06432922574812154</v>
+        <v>-0.06432922574812137</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.05220627135387298</v>
+        <v>-0.05220627135387299</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0760657367823839</v>
+        <v>0.07606573678238433</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.08360957169362965</v>
+        <v>-0.08360957169362936</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0120577283038844</v>
+        <v>-0.01205772830388437</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.05465711834592554</v>
+        <v>-0.0546571183459256</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.103698342794782</v>
+        <v>-0.1036983427947809</v>
       </c>
       <c r="R21" t="n">
-        <v>0.03637625638365085</v>
+        <v>0.03637625638365086</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.1100962586465691</v>
+        <v>-0.1100962586465682</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.006222482790362939</v>
+        <v>-0.006222482790362905</v>
       </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
-        <v>-0.0949068552938693</v>
+        <v>-0.09490685529386887</v>
       </c>
       <c r="W21" t="n">
-        <v>-0.08993315044937295</v>
+        <v>-0.08993315044937226</v>
       </c>
       <c r="X21" t="n">
-        <v>0.05137300356690729</v>
+        <v>0.05137300356690742</v>
       </c>
       <c r="Y21" t="n">
-        <v>-0.04572244115179949</v>
+        <v>-0.04572244115179931</v>
       </c>
       <c r="Z21" t="n">
-        <v>-0.09735367517730985</v>
+        <v>-0.09735367517730913</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.1054395755929265</v>
+        <v>0.1054395755929252</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.01411537834941107</v>
+        <v>-0.01411537834941089</v>
       </c>
       <c r="AC21" t="n">
-        <v>-0.119148661185463</v>
+        <v>-0.1191486611854633</v>
       </c>
       <c r="AD21" t="n">
-        <v>-0.0115073652370464</v>
+        <v>-0.01150736523704633</v>
       </c>
     </row>
     <row r="22">
@@ -2467,91 +2467,91 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.009497326623880441</v>
+        <v>0.009497326623859647</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02781125497952122</v>
+        <v>0.02781125497952166</v>
       </c>
       <c r="D22" t="n">
-        <v>0.03663948474760154</v>
+        <v>0.03663948474760128</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.009927045468401442</v>
+        <v>-0.009927045468401587</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.1089322791113146</v>
+        <v>-0.1089322791113128</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.03178511420970341</v>
+        <v>-0.0317851142097036</v>
       </c>
       <c r="H22" t="n">
-        <v>0.08150582366447642</v>
+        <v>0.08150582366447644</v>
       </c>
       <c r="I22" t="n">
-        <v>0.03914221414788874</v>
+        <v>0.0391422141478881</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.01492358163074485</v>
+        <v>-0.01492358163074341</v>
       </c>
       <c r="K22" t="n">
-        <v>0.07419310337784693</v>
+        <v>0.07419310337784719</v>
       </c>
       <c r="L22" t="n">
-        <v>0.05862524183523384</v>
+        <v>0.05862524183523415</v>
       </c>
       <c r="M22" t="n">
-        <v>0.03624412638198279</v>
+        <v>0.03624412638198244</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2769890893549909</v>
+        <v>0.2769890893549882</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.05007367349742455</v>
+        <v>-0.0500736734974245</v>
       </c>
       <c r="P22" t="n">
-        <v>0.04578199743103132</v>
+        <v>0.04578199743103103</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.001158733198858472</v>
+        <v>0.001158733198858716</v>
       </c>
       <c r="R22" t="n">
-        <v>-0.04523204088140949</v>
+        <v>-0.04523204088140973</v>
       </c>
       <c r="S22" t="n">
-        <v>0.007222014700928866</v>
+        <v>0.007222014700928612</v>
       </c>
       <c r="T22" t="n">
         <v>-0.01596469403155534</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.0949068552938693</v>
+        <v>-0.09490685529386887</v>
       </c>
       <c r="V22" t="n">
         <v>1</v>
       </c>
       <c r="W22" t="n">
-        <v>0.008672548460993615</v>
+        <v>0.008672548460993218</v>
       </c>
       <c r="X22" t="n">
-        <v>0.02507139153947508</v>
+        <v>0.02507139153947497</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.1948479959017639</v>
+        <v>0.194847995901764</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.06574572525098814</v>
+        <v>0.06574572525098911</v>
       </c>
       <c r="AA22" t="n">
-        <v>-0.06501755382351464</v>
+        <v>-0.06501755382351436</v>
       </c>
       <c r="AB22" t="n">
-        <v>-0.03042291402674992</v>
+        <v>-0.03042291402674981</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.03357945472237968</v>
+        <v>0.03357945472238019</v>
       </c>
       <c r="AD22" t="n">
-        <v>-0.01035051011862847</v>
+        <v>-0.01035051011862836</v>
       </c>
     </row>
     <row r="23">
@@ -2561,91 +2561,91 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.002941432585387207</v>
+        <v>0.00294143258538511</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04481943691241007</v>
+        <v>0.04481943691241014</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.108249922874552</v>
+        <v>-0.1082499228745516</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1857402266390834</v>
+        <v>0.1857402266390846</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.09901520957341113</v>
+        <v>-0.09901520957340881</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.09664702363980325</v>
+        <v>-0.09664702363980367</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02306022491483493</v>
+        <v>0.02306022491483497</v>
       </c>
       <c r="I23" t="n">
-        <v>0.05948459823898868</v>
+        <v>0.05948459823898915</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.1715391509211246</v>
+        <v>-0.1715391509211264</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.1234197914188628</v>
+        <v>-0.123419791418862</v>
       </c>
       <c r="L23" t="n">
-        <v>0.03897303022562307</v>
+        <v>0.03897303022562335</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.1375542232090765</v>
+        <v>-0.1375542232090763</v>
       </c>
       <c r="N23" t="n">
-        <v>0.005493622971748061</v>
+        <v>0.005493622971748255</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.001486675404982053</v>
+        <v>-0.001486675404982047</v>
       </c>
       <c r="P23" t="n">
-        <v>0.002483263557514506</v>
+        <v>0.002483263557514441</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.03767108432824334</v>
+        <v>0.03767108432824318</v>
       </c>
       <c r="R23" t="n">
-        <v>0.02985138372821214</v>
+        <v>0.02985138372821246</v>
       </c>
       <c r="S23" t="n">
-        <v>0.3806254518602876</v>
+        <v>0.3806254518602838</v>
       </c>
       <c r="T23" t="n">
-        <v>-0.1145480770662133</v>
+        <v>-0.1145480770662147</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.08993315044937295</v>
+        <v>-0.08993315044937226</v>
       </c>
       <c r="V23" t="n">
-        <v>0.008672548460993615</v>
+        <v>0.008672548460993218</v>
       </c>
       <c r="W23" t="n">
         <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>-0.03439743460397043</v>
+        <v>-0.03439743460397045</v>
       </c>
       <c r="Y23" t="n">
-        <v>-0.03992561052943552</v>
+        <v>-0.03992561052943582</v>
       </c>
       <c r="Z23" t="n">
-        <v>-0.1239194396450397</v>
+        <v>-0.1239194396450401</v>
       </c>
       <c r="AA23" t="n">
-        <v>-0.06425196938889512</v>
+        <v>-0.06425196938889448</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.04177486228621299</v>
+        <v>-0.04177486228621325</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.1138778076145074</v>
+        <v>0.113877807614507</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.003535987999010686</v>
+        <v>-0.003535987999010713</v>
       </c>
     </row>
     <row r="24">
@@ -2655,91 +2655,91 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.005003910971445519</v>
+        <v>0.005003910971446085</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.0358605225742939</v>
+        <v>-0.03586052257429424</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.06455220261611155</v>
+        <v>-0.06455220261611073</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01048213081496958</v>
+        <v>0.0104821308149696</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0735867004219814</v>
+        <v>0.07358670042198172</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04811196699130712</v>
+        <v>0.0481119669913073</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.07774297094939014</v>
+        <v>-0.07774297094939057</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2163664193155172</v>
+        <v>0.2163664193155169</v>
       </c>
       <c r="J24" t="n">
-        <v>0.004669191514804919</v>
+        <v>0.004669191514805735</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01160106055080734</v>
+        <v>0.01160106055080736</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.07304035230077455</v>
+        <v>-0.07304035230077466</v>
       </c>
       <c r="M24" t="n">
-        <v>0.01943064813602756</v>
+        <v>0.01943064813602745</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0282435271655872</v>
+        <v>0.02824352716558755</v>
       </c>
       <c r="O24" t="n">
-        <v>0.02387392725260601</v>
+        <v>0.02387392725260604</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.05720384552394039</v>
+        <v>-0.05720384552394082</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.1315965272369784</v>
+        <v>-0.1315965272369776</v>
       </c>
       <c r="R24" t="n">
-        <v>0.07424054917440119</v>
+        <v>0.07424054917440127</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.04302614111301012</v>
+        <v>-0.04302614111301006</v>
       </c>
       <c r="T24" t="n">
-        <v>0.04166142694064974</v>
+        <v>0.04166142694064977</v>
       </c>
       <c r="U24" t="n">
-        <v>0.05137300356690729</v>
+        <v>0.05137300356690742</v>
       </c>
       <c r="V24" t="n">
-        <v>0.02507139153947508</v>
+        <v>0.02507139153947497</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.03439743460397043</v>
+        <v>-0.03439743460397045</v>
       </c>
       <c r="X24" t="n">
         <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.01772476306817743</v>
+        <v>0.01772476306817729</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.03673256970492839</v>
+        <v>-0.03673256970492826</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.09592645206485106</v>
+        <v>0.0959264520648508</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.01631311760248445</v>
+        <v>-0.01631311760248449</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.1278918315237323</v>
+        <v>-0.1278918315237322</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.00486480594013578</v>
+        <v>-0.004864805940135796</v>
       </c>
     </row>
     <row r="25">
@@ -2749,91 +2749,91 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0008010430298418943</v>
+        <v>0.0008010430298134766</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0125200163497233</v>
+        <v>0.01252001634972355</v>
       </c>
       <c r="D25" t="n">
-        <v>0.08380594414087883</v>
+        <v>0.08380594414087869</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.06123995584416253</v>
+        <v>-0.06123995584416318</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.04788222386583905</v>
+        <v>-0.04788222386583824</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01688105226224058</v>
+        <v>0.0168810522622406</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06837757927492207</v>
+        <v>0.06837757927492243</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.001998790661104619</v>
+        <v>-0.001998790661104742</v>
       </c>
       <c r="J25" t="n">
-        <v>0.04132731441204203</v>
+        <v>0.04132731441204204</v>
       </c>
       <c r="K25" t="n">
-        <v>0.08432036723016692</v>
+        <v>0.0843203672301677</v>
       </c>
       <c r="L25" t="n">
-        <v>0.05257813613734239</v>
+        <v>0.05257813613734297</v>
       </c>
       <c r="M25" t="n">
-        <v>0.06490096721177657</v>
+        <v>0.06490096721177659</v>
       </c>
       <c r="N25" t="n">
-        <v>0.3171485346167666</v>
+        <v>0.3171485346167626</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.02634277216924626</v>
+        <v>-0.02634277216924662</v>
       </c>
       <c r="P25" t="n">
-        <v>0.07505107035809126</v>
+        <v>0.07505107035809171</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.001188264917783325</v>
+        <v>0.001188264917783762</v>
       </c>
       <c r="R25" t="n">
-        <v>-0.02442188641142188</v>
+        <v>-0.02442188641142184</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.03899381807571244</v>
+        <v>-0.03899381807571276</v>
       </c>
       <c r="T25" t="n">
-        <v>-0.007910229573284319</v>
+        <v>-0.00791022957328465</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.04572244115179949</v>
+        <v>-0.04572244115179931</v>
       </c>
       <c r="V25" t="n">
-        <v>0.1948479959017639</v>
+        <v>0.194847995901764</v>
       </c>
       <c r="W25" t="n">
-        <v>-0.03992561052943552</v>
+        <v>-0.03992561052943582</v>
       </c>
       <c r="X25" t="n">
-        <v>0.01772476306817743</v>
+        <v>0.01772476306817729</v>
       </c>
       <c r="Y25" t="n">
         <v>1</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.05814250555685055</v>
+        <v>0.05814250555685131</v>
       </c>
       <c r="AA25" t="n">
-        <v>-0.0306882798565359</v>
+        <v>-0.03068827985653607</v>
       </c>
       <c r="AB25" t="n">
-        <v>-0.02580622794139137</v>
+        <v>-0.02580622794139138</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.006063364069331491</v>
+        <v>0.00606336406933179</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.01023912269725002</v>
+        <v>0.01023912269725023</v>
       </c>
     </row>
     <row r="26">
@@ -2843,91 +2843,91 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.009408097150033124</v>
+        <v>-0.009408097150011193</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.003483363700039387</v>
+        <v>-0.003483363700040023</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2568660344935288</v>
+        <v>0.2568660344935301</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.1421976854004575</v>
+        <v>-0.1421976854004574</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.1206321809120469</v>
+        <v>-0.1206321809120477</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.05101035330868532</v>
+        <v>-0.05101035330868514</v>
       </c>
       <c r="H26" t="n">
-        <v>0.06111048046672673</v>
+        <v>0.06111048046672687</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.08980249677434633</v>
+        <v>-0.08980249677434596</v>
       </c>
       <c r="J26" t="n">
-        <v>0.418628273139914</v>
+        <v>0.418628273139917</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4193997560018932</v>
+        <v>0.4193997560018921</v>
       </c>
       <c r="L26" t="n">
-        <v>0.09762831260398865</v>
+        <v>0.09762831260398891</v>
       </c>
       <c r="M26" t="n">
-        <v>0.2946619357661486</v>
+        <v>0.294661935766147</v>
       </c>
       <c r="N26" t="n">
-        <v>0.03975230575459605</v>
+        <v>0.03975230575459551</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.2733345542053867</v>
+        <v>-0.273334554205385</v>
       </c>
       <c r="P26" t="n">
-        <v>0.1967676808498771</v>
+        <v>0.1967676808498794</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.09736058552479951</v>
+        <v>0.09736058552480011</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.1364583303218727</v>
+        <v>-0.1364583303218744</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.190701823841399</v>
+        <v>-0.1907018238413989</v>
       </c>
       <c r="T26" t="n">
-        <v>-0.04008735733789851</v>
+        <v>-0.04008735733789861</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.09735367517730985</v>
+        <v>-0.09735367517730913</v>
       </c>
       <c r="V26" t="n">
-        <v>0.06574572525098814</v>
+        <v>0.06574572525098911</v>
       </c>
       <c r="W26" t="n">
-        <v>-0.1239194396450397</v>
+        <v>-0.1239194396450401</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.03673256970492839</v>
+        <v>-0.03673256970492826</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.05814250555685055</v>
+        <v>0.05814250555685131</v>
       </c>
       <c r="Z26" t="n">
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>-0.06669705207424843</v>
+        <v>-0.06669705207424759</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.006869661419212267</v>
+        <v>0.006869661419212199</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.06741003509163668</v>
+        <v>0.06741003509163665</v>
       </c>
       <c r="AD26" t="n">
-        <v>-0.001824929626409258</v>
+        <v>-0.001824929626409422</v>
       </c>
     </row>
     <row r="27">
@@ -2937,91 +2937,91 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.005426099532319422</v>
+        <v>0.005426099532313172</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.0661294438138972</v>
+        <v>-0.06612944381389659</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.02677572435974179</v>
+        <v>-0.02677572435974134</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.050870085872</v>
+        <v>-0.05087008587199935</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1230084554100962</v>
+        <v>0.1230084554100948</v>
       </c>
       <c r="G27" t="n">
-        <v>0.09573980675138695</v>
+        <v>0.09573980675138585</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.2779357062449836</v>
+        <v>-0.2779357062449813</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01072743307583247</v>
+        <v>0.01072743307583234</v>
       </c>
       <c r="J27" t="n">
-        <v>0.03807358625458564</v>
+        <v>0.03807358625458487</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.0180122360040814</v>
+        <v>-0.01801223600408141</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.1584801244511929</v>
+        <v>-0.1584801244511936</v>
       </c>
       <c r="M27" t="n">
-        <v>0.04040243838788284</v>
+        <v>0.04040243838788274</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.03988356159728796</v>
+        <v>-0.03988356159728736</v>
       </c>
       <c r="O27" t="n">
-        <v>0.05745802077997252</v>
+        <v>0.05745802077997238</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.02532082955913875</v>
+        <v>-0.02532082955913859</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.179934843894821</v>
+        <v>-0.1799348438948209</v>
       </c>
       <c r="R27" t="n">
-        <v>0.1970722535658273</v>
+        <v>0.1970722535658275</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.07509590136447311</v>
+        <v>-0.07509590136447344</v>
       </c>
       <c r="T27" t="n">
-        <v>0.2649765140623815</v>
+        <v>0.2649765140623843</v>
       </c>
       <c r="U27" t="n">
-        <v>0.1054395755929265</v>
+        <v>0.1054395755929252</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.06501755382351464</v>
+        <v>-0.06501755382351436</v>
       </c>
       <c r="W27" t="n">
-        <v>-0.06425196938889512</v>
+        <v>-0.06425196938889448</v>
       </c>
       <c r="X27" t="n">
-        <v>0.09592645206485106</v>
+        <v>0.0959264520648508</v>
       </c>
       <c r="Y27" t="n">
-        <v>-0.0306882798565359</v>
+        <v>-0.03068827985653607</v>
       </c>
       <c r="Z27" t="n">
-        <v>-0.06669705207424843</v>
+        <v>-0.06669705207424759</v>
       </c>
       <c r="AA27" t="n">
         <v>1</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.1236080503189724</v>
+        <v>0.1236080503189705</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.3039817849297376</v>
+        <v>-0.3039817849297362</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.007492864367658309</v>
+        <v>0.007492864367658199</v>
       </c>
     </row>
     <row r="28">
@@ -3031,91 +3031,91 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.004392818585108896</v>
+        <v>-0.004392818585115982</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01355440587483009</v>
+        <v>0.01355440587483</v>
       </c>
       <c r="D28" t="n">
-        <v>0.04137257711003997</v>
+        <v>0.04137257711004026</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.07113979528195961</v>
+        <v>-0.07113979528195999</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.03274846807870283</v>
+        <v>-0.03274846807870237</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0109430165515314</v>
+        <v>0.01094301655153136</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.04252764104902889</v>
+        <v>-0.0425276410490285</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.1566592073495101</v>
+        <v>-0.1566592073495103</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.02671046812049865</v>
+        <v>-0.02671046812049771</v>
       </c>
       <c r="K28" t="n">
-        <v>0.01440263580629536</v>
+        <v>0.01440263580629541</v>
       </c>
       <c r="L28" t="n">
-        <v>0.04897913315473101</v>
+        <v>0.04897913315473058</v>
       </c>
       <c r="M28" t="n">
-        <v>0.02113975537609423</v>
+        <v>0.02113975537609375</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.01023285931755934</v>
+        <v>-0.01023285931755932</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0006378176445430204</v>
+        <v>0.0006378176445429979</v>
       </c>
       <c r="P28" t="n">
-        <v>0.100842758956742</v>
+        <v>0.1008427589567406</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.01928345916355061</v>
+        <v>0.01928345916355012</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.01723209823915177</v>
+        <v>-0.01723209823915158</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.04155875220409582</v>
+        <v>-0.04155875220409568</v>
       </c>
       <c r="T28" t="n">
-        <v>0.3991755876204435</v>
+        <v>0.399175587620446</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.01411537834941107</v>
+        <v>-0.01411537834941089</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.03042291402674992</v>
+        <v>-0.03042291402674981</v>
       </c>
       <c r="W28" t="n">
-        <v>-0.04177486228621299</v>
+        <v>-0.04177486228621325</v>
       </c>
       <c r="X28" t="n">
-        <v>-0.01631311760248445</v>
+        <v>-0.01631311760248449</v>
       </c>
       <c r="Y28" t="n">
-        <v>-0.02580622794139137</v>
+        <v>-0.02580622794139138</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.006869661419212267</v>
+        <v>0.006869661419212199</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.1236080503189724</v>
+        <v>0.1236080503189705</v>
       </c>
       <c r="AB28" t="n">
         <v>1</v>
       </c>
       <c r="AC28" t="n">
-        <v>-0.09880866491964323</v>
+        <v>-0.09880866491964305</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.008762422081588672</v>
+        <v>-0.0087624220815885</v>
       </c>
     </row>
     <row r="29">
@@ -3125,91 +3125,91 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.01082710065890249</v>
+        <v>-0.01082710065890333</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0842009076313234</v>
+        <v>0.084200907631323</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01170716638941764</v>
+        <v>0.01170716638941757</v>
       </c>
       <c r="E29" t="n">
-        <v>0.08153572737599171</v>
+        <v>0.0815357273759923</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.1495979406489653</v>
+        <v>-0.1495979406489637</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.1613721687741418</v>
+        <v>-0.161372168774144</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1849532431283435</v>
+        <v>0.1849532431283424</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02058144507498665</v>
+        <v>-0.02058144507498651</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0283806244469918</v>
+        <v>-0.02838062444699174</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.01724922605509063</v>
+        <v>-0.01724922605509062</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1466866568400325</v>
+        <v>0.1466866568400333</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.08553931658610751</v>
+        <v>-0.08553931658610614</v>
       </c>
       <c r="N29" t="n">
-        <v>0.01462849170605041</v>
+        <v>0.01462849170605009</v>
       </c>
       <c r="O29" t="n">
-        <v>-0.04060749642768548</v>
+        <v>-0.04060749642768538</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.005912817915373824</v>
+        <v>-0.005912817915373845</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.2774237764659984</v>
+        <v>0.2774237764659986</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.1640239568781148</v>
+        <v>-0.1640239568781167</v>
       </c>
       <c r="S29" t="n">
-        <v>0.1281674556597141</v>
+        <v>0.1281674556597133</v>
       </c>
       <c r="T29" t="n">
-        <v>-0.2752613552520654</v>
+        <v>-0.2752613552520646</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.119148661185463</v>
+        <v>-0.1191486611854633</v>
       </c>
       <c r="V29" t="n">
-        <v>0.03357945472237968</v>
+        <v>0.03357945472238019</v>
       </c>
       <c r="W29" t="n">
-        <v>0.1138778076145074</v>
+        <v>0.113877807614507</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.1278918315237323</v>
+        <v>-0.1278918315237322</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.006063364069331491</v>
+        <v>0.00606336406933179</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.06741003509163668</v>
+        <v>0.06741003509163665</v>
       </c>
       <c r="AA29" t="n">
-        <v>-0.3039817849297376</v>
+        <v>-0.3039817849297362</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.09880866491964323</v>
+        <v>-0.09880866491964305</v>
       </c>
       <c r="AC29" t="n">
         <v>1</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.01329528552794513</v>
+        <v>-0.01329528552794521</v>
       </c>
     </row>
     <row r="30">
@@ -3225,82 +3225,82 @@
         <v>0.0106089585031679</v>
       </c>
       <c r="D30" t="n">
-        <v>0.004544723741324455</v>
+        <v>0.00454472374132441</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.009027057405997655</v>
+        <v>-0.009027057405997772</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001918246918019292</v>
+        <v>0.001918246918019185</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0004213666633361417</v>
+        <v>0.000421366663336117</v>
       </c>
       <c r="H30" t="n">
-        <v>0.005426109759395114</v>
+        <v>0.005426109759395126</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.007568510999958534</v>
+        <v>-0.007568510999958596</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.008696629340338607</v>
+        <v>-0.008696629340339374</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.004571282443345222</v>
+        <v>-0.004571282443345205</v>
       </c>
       <c r="L30" t="n">
-        <v>0.005873925907306311</v>
+        <v>0.005873925907306308</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.01594584507032234</v>
+        <v>-0.01594584507032239</v>
       </c>
       <c r="N30" t="n">
-        <v>-0.004039404939309665</v>
+        <v>-0.00403940493930977</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.004234008957905645</v>
+        <v>-0.004234008957905523</v>
       </c>
       <c r="P30" t="n">
-        <v>0.001272051356885027</v>
+        <v>0.001272051356885095</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.004219300638306392</v>
+        <v>0.004219300638306309</v>
       </c>
       <c r="R30" t="n">
-        <v>0.004214917736628397</v>
+        <v>0.004214917736628346</v>
       </c>
       <c r="S30" t="n">
-        <v>0.005855144767080881</v>
+        <v>0.005855144767080836</v>
       </c>
       <c r="T30" t="n">
-        <v>-0.0003191464164218632</v>
+        <v>-0.0003191464164218972</v>
       </c>
       <c r="U30" t="n">
-        <v>-0.0115073652370464</v>
+        <v>-0.01150736523704633</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.01035051011862847</v>
+        <v>-0.01035051011862836</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.003535987999010686</v>
+        <v>-0.003535987999010713</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.00486480594013578</v>
+        <v>-0.004864805940135796</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.01023912269725002</v>
+        <v>0.01023912269725023</v>
       </c>
       <c r="Z30" t="n">
-        <v>-0.001824929626409258</v>
+        <v>-0.001824929626409422</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.007492864367658309</v>
+        <v>0.007492864367658199</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.008762422081588672</v>
+        <v>-0.0087624220815885</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.01329528552794513</v>
+        <v>-0.01329528552794521</v>
       </c>
       <c r="AD30" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Selected Standardization and kNN Imputer
</commit_message>
<xml_diff>
--- a/CaseStudy/Export/Correlation.xlsx
+++ b/CaseStudy/Export/Correlation.xlsx
@@ -593,82 +593,82 @@
         <v>-0.007008472659042641</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.005070223811738058</v>
+        <v>-0.005070223811740497</v>
       </c>
       <c r="E2" t="n">
-        <v>0.007199714812957908</v>
+        <v>0.007199714812955446</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0007085235742506061</v>
+        <v>-0.0007085235742571006</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001996650017357398</v>
+        <v>0.001996650017355911</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.01344581076908015</v>
+        <v>-0.01344581076908236</v>
       </c>
       <c r="I2" t="n">
-        <v>0.005327843942331428</v>
+        <v>0.005327843942332374</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.006751821148425145</v>
+        <v>-0.006751821148455144</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.004841507045589334</v>
+        <v>-0.004841507045589901</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.003810115400934034</v>
+        <v>-0.003810115400934361</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.007806676320152247</v>
+        <v>-0.007806676320154338</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.001954009510615686</v>
+        <v>-0.00195400951064774</v>
       </c>
       <c r="O2" t="n">
-        <v>0.005819122517392793</v>
+        <v>0.005819122517400661</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.008440869839978979</v>
+        <v>-0.008440869839974762</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.01582495487227976</v>
+        <v>-0.0158249548722751</v>
       </c>
       <c r="R2" t="n">
-        <v>0.002415649425692551</v>
+        <v>0.002415649425689274</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.0009807823932814451</v>
+        <v>-0.0009807823932810756</v>
       </c>
       <c r="T2" t="n">
-        <v>0.003911157232878403</v>
+        <v>0.003911157232875786</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0005967040528228183</v>
+        <v>0.0005967040528196539</v>
       </c>
       <c r="V2" t="n">
-        <v>0.009497326623859647</v>
+        <v>0.009497326623880427</v>
       </c>
       <c r="W2" t="n">
-        <v>0.00294143258538511</v>
+        <v>0.002941432585387215</v>
       </c>
       <c r="X2" t="n">
-        <v>0.005003910971446085</v>
+        <v>0.005003910971445515</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0008010430298134766</v>
+        <v>0.0008010430298419018</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.009408097150011193</v>
+        <v>-0.009408097150033113</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.005426099532313172</v>
+        <v>0.005426099532319414</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.004392818585115982</v>
+        <v>-0.004392818585108846</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.01082710065890333</v>
+        <v>-0.01082710065890251</v>
       </c>
       <c r="AD2" t="n">
         <v>-0.007993536627121576</v>
@@ -687,82 +687,82 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05044208461916696</v>
+        <v>0.05044208461916677</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06779927667853999</v>
+        <v>0.06779927667853981</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.04645467609019886</v>
+        <v>-0.04645467609019995</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.01877136399188564</v>
+        <v>-0.01877136399188553</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1347852553956619</v>
+        <v>0.1347852553956621</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.05595703662236306</v>
+        <v>-0.055957036622363</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.06700792996032565</v>
+        <v>-0.06700792996032622</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.02412574075441339</v>
+        <v>-0.02412574075441358</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0567146391968809</v>
+        <v>0.05671463919688057</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.02621911321679688</v>
+        <v>-0.02621911321679693</v>
       </c>
       <c r="N3" t="n">
-        <v>0.02516347794757303</v>
+        <v>0.02516347794757306</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.002006199593661507</v>
+        <v>-0.002006199593661595</v>
       </c>
       <c r="P3" t="n">
-        <v>0.04407645986771008</v>
+        <v>0.04407645986770938</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1189735699689563</v>
+        <v>0.1189735699689564</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.04221801463848525</v>
+        <v>-0.04221801463848573</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0703432573653735</v>
+        <v>0.07034325736537461</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.003794108679387379</v>
+        <v>-0.003794108679387351</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.0457864802152591</v>
+        <v>-0.04578648021525925</v>
       </c>
       <c r="V3" t="n">
-        <v>0.02781125497952166</v>
+        <v>0.02781125497952147</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04481943691241014</v>
+        <v>0.04481943691241003</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.03586052257429424</v>
+        <v>-0.03586052257429406</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.01252001634972355</v>
+        <v>0.01252001634972327</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.003483363700040023</v>
+        <v>-0.003483363700039383</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.06612944381389659</v>
+        <v>-0.06612944381389728</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.01355440587483</v>
+        <v>0.01355440587483003</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.084200907631323</v>
+        <v>0.0842009076313236</v>
       </c>
       <c r="AD3" t="n">
         <v>0.0106089585031679</v>
@@ -775,91 +775,91 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.005070223811738058</v>
+        <v>-0.005070223811740497</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05044208461916696</v>
+        <v>0.05044208461916677</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2854228459919291</v>
+        <v>-0.2854228459919292</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03876588119624808</v>
+        <v>0.03876588119624899</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1031036205733086</v>
+        <v>0.1031036205733095</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02506768403700984</v>
+        <v>0.02506768403701007</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.1240683217221154</v>
+        <v>-0.1240683217221146</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2015400208497256</v>
+        <v>0.2015400208497262</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2244892493389906</v>
+        <v>0.2244892493389938</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1277295672132354</v>
+        <v>0.1277295672132343</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2335739591475398</v>
+        <v>0.2335739591475378</v>
       </c>
       <c r="N4" t="n">
-        <v>0.04104506306654939</v>
+        <v>0.04104506306654923</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.1093791755856592</v>
+        <v>-0.1093791755856588</v>
       </c>
       <c r="P4" t="n">
         <v>0.2134837274346892</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1232799394661991</v>
+        <v>0.1232799394662006</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.2211626770849093</v>
+        <v>-0.2211626770849112</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.1342813671830702</v>
+        <v>-0.1342813671830735</v>
       </c>
       <c r="T4" t="n">
-        <v>0.03189711144304377</v>
+        <v>0.03189711144304385</v>
       </c>
       <c r="U4" t="n">
-        <v>0.05370476839399391</v>
+        <v>0.05370476839399382</v>
       </c>
       <c r="V4" t="n">
-        <v>0.03663948474760128</v>
+        <v>0.03663948474760147</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.1082499228745516</v>
+        <v>-0.1082499228745526</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.06455220261611073</v>
+        <v>-0.06455220261611086</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.08380594414087869</v>
+        <v>0.08380594414087833</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2568660344935301</v>
+        <v>0.25686603449353</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.02677572435974134</v>
+        <v>-0.02677572435974145</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.04137257711004026</v>
+        <v>0.04137257711004009</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.01170716638941757</v>
+        <v>0.01170716638941756</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.00454472374132441</v>
+        <v>0.004544723741324472</v>
       </c>
     </row>
     <row r="5">
@@ -869,91 +869,91 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.007199714812957908</v>
+        <v>0.007199714812955446</v>
       </c>
       <c r="C5" t="n">
-        <v>0.06779927667853999</v>
+        <v>0.06779927667853981</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2854228459919291</v>
+        <v>-0.2854228459919292</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1659442236438829</v>
+        <v>-0.1659442236438831</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1915984574506099</v>
+        <v>-0.1915984574506089</v>
       </c>
       <c r="H5" t="n">
-        <v>0.03178008536421191</v>
+        <v>0.0317800853642119</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1332431641180928</v>
+        <v>0.1332431641180914</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.1588929993566444</v>
+        <v>-0.1588929993566437</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1359016179997409</v>
+        <v>-0.1359016179997426</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.09482163926037218</v>
+        <v>-0.09482163926037185</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1841377598445468</v>
+        <v>-0.1841377598445477</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.01823123135068524</v>
+        <v>-0.01823123135068552</v>
       </c>
       <c r="O5" t="n">
-        <v>0.06488022195694104</v>
+        <v>0.06488022195694118</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1610312267027513</v>
+        <v>-0.1610312267027528</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.06471908231036244</v>
+        <v>-0.0647190823103629</v>
       </c>
       <c r="R5" t="n">
-        <v>0.2137294667945424</v>
+        <v>0.2137294667945406</v>
       </c>
       <c r="S5" t="n">
-        <v>0.2404141307388312</v>
+        <v>0.2404141307388295</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.08699327581894981</v>
+        <v>-0.08699327581894925</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.1647399506653912</v>
+        <v>-0.1647399506653904</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.009927045468401587</v>
+        <v>-0.009927045468401514</v>
       </c>
       <c r="W5" t="n">
-        <v>0.1857402266390846</v>
+        <v>0.1857402266390854</v>
       </c>
       <c r="X5" t="n">
-        <v>0.0104821308149696</v>
+        <v>0.01048213081496965</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.06123995584416318</v>
+        <v>-0.06123995584416266</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.1421976854004574</v>
+        <v>-0.142197685400458</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.05087008587199935</v>
+        <v>-0.05087008587199974</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.07113979528195999</v>
+        <v>-0.07113979528195946</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.0815357273759923</v>
+        <v>0.08153572737599282</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.009027057405997772</v>
+        <v>-0.009027057405997746</v>
       </c>
     </row>
     <row r="6">
@@ -963,91 +963,91 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0007085235742506061</v>
+        <v>-0.0007085235742571006</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.04645467609019886</v>
+        <v>-0.04645467609019995</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03876588119624808</v>
+        <v>0.03876588119624899</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1659442236438829</v>
+        <v>-0.1659442236438831</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3937092311458016</v>
+        <v>0.3937092311458065</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1647710451171668</v>
+        <v>-0.1647710451171696</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06749129753345921</v>
+        <v>0.06749129753345887</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0867731770612358</v>
+        <v>0.08677317706123683</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.08367488681719192</v>
+        <v>-0.08367488681719261</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.06399826795457438</v>
+        <v>-0.06399826795457476</v>
       </c>
       <c r="M6" t="n">
-        <v>0.06695412066191682</v>
+        <v>0.066954120661917</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0910335862665629</v>
+        <v>-0.09103358626656365</v>
       </c>
       <c r="O6" t="n">
-        <v>0.00817052050051075</v>
+        <v>0.00817052050051083</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.06132815058585541</v>
+        <v>-0.0613281505858554</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.1424848395321638</v>
+        <v>-0.142484839532166</v>
       </c>
       <c r="R6" t="n">
-        <v>0.05363510207263694</v>
+        <v>0.05363510207263771</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.1108649630770478</v>
+        <v>-0.1108649630770486</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.005657214339024754</v>
+        <v>-0.005657214339024872</v>
       </c>
       <c r="U6" t="n">
-        <v>0.5163389916032641</v>
+        <v>0.5163389916032668</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1089322791113128</v>
+        <v>-0.108932279111314</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.09901520957340881</v>
+        <v>-0.09901520957341101</v>
       </c>
       <c r="X6" t="n">
-        <v>0.07358670042198172</v>
+        <v>0.07358670042198175</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.04788222386583824</v>
+        <v>-0.04788222386583884</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.1206321809120477</v>
+        <v>-0.1206321809120494</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1230084554100948</v>
+        <v>0.123008455410096</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.03274846807870237</v>
+        <v>-0.03274846807870244</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.1495979406489637</v>
+        <v>-0.1495979406489656</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.001918246918019185</v>
+        <v>0.001918246918019261</v>
       </c>
     </row>
     <row r="7">
@@ -1057,91 +1057,91 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001996650017357398</v>
+        <v>0.001996650017355911</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.01877136399188564</v>
+        <v>-0.01877136399188553</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1031036205733086</v>
+        <v>0.1031036205733095</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1915984574506099</v>
+        <v>-0.1915984574506089</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3937092311458016</v>
+        <v>0.3937092311458065</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.01744445223407567</v>
+        <v>-0.01744445223407552</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.01110522927200634</v>
+        <v>-0.01110522927200638</v>
       </c>
       <c r="J7" t="n">
-        <v>0.09359933008622667</v>
+        <v>0.09359933008622548</v>
       </c>
       <c r="K7" t="n">
-        <v>0.04884581038940265</v>
+        <v>0.04884581038940244</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.06480089222744193</v>
+        <v>-0.06480089222744131</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2183685993399871</v>
+        <v>0.2183685993399875</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.0110671685484269</v>
+        <v>-0.01106716854842708</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.061446475280487</v>
+        <v>-0.06144647528048627</v>
       </c>
       <c r="P7" t="n">
-        <v>0.05745204772809384</v>
+        <v>0.05745204772809313</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.1017707294568489</v>
+        <v>-0.1017707294568498</v>
       </c>
       <c r="R7" t="n">
-        <v>0.08547959274002555</v>
+        <v>0.08547959274002463</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.1396715866169304</v>
+        <v>-0.1396715866169305</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1474424934269196</v>
+        <v>0.1474424934269187</v>
       </c>
       <c r="U7" t="n">
-        <v>0.376969338478802</v>
+        <v>0.3769693384788039</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.0317851142097036</v>
+        <v>-0.0317851142097037</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.09664702363980367</v>
+        <v>-0.0966470236398032</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0481119669913073</v>
+        <v>0.04811196699130717</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.0168810522622406</v>
+        <v>0.01688105226224053</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.05101035330868514</v>
+        <v>-0.05101035330868505</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.09573980675138585</v>
+        <v>0.0957398067513857</v>
       </c>
       <c r="AB7" t="n">
         <v>0.01094301655153136</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.161372168774144</v>
+        <v>-0.1613721687741443</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.000421366663336117</v>
+        <v>0.0004213666633361352</v>
       </c>
     </row>
     <row r="8">
@@ -1151,91 +1151,91 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.01344581076908015</v>
+        <v>-0.01344581076908236</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1347852553956619</v>
+        <v>0.1347852553956621</v>
       </c>
       <c r="D8" t="n">
-        <v>0.02506768403700984</v>
+        <v>0.02506768403701007</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03178008536421191</v>
+        <v>0.0317800853642119</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1647710451171668</v>
+        <v>-0.1647710451171696</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01744445223407567</v>
+        <v>-0.01744445223407552</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.1025703582654423</v>
+        <v>-0.1025703582654421</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.08882547027173492</v>
+        <v>-0.08882547027173518</v>
       </c>
       <c r="K8" t="n">
-        <v>0.03967748778025364</v>
+        <v>0.03967748778025409</v>
       </c>
       <c r="L8" t="n">
-        <v>0.143380904978012</v>
+        <v>0.1433809049780099</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01006404030103045</v>
+        <v>0.01006404030103051</v>
       </c>
       <c r="N8" t="n">
-        <v>0.06650253986622809</v>
+        <v>0.0665025398662283</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.08329810050424556</v>
+        <v>-0.08329810050424651</v>
       </c>
       <c r="P8" t="n">
-        <v>0.08274365449228922</v>
+        <v>0.0827436544922879</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2116712719142572</v>
+        <v>0.2116712719142609</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1602828742365812</v>
+        <v>-0.1602828742365819</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04686897793799374</v>
+        <v>0.04686897793799358</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.1027593134180955</v>
+        <v>-0.1027593134180966</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.1563366399626703</v>
+        <v>-0.1563366399626698</v>
       </c>
       <c r="V8" t="n">
-        <v>0.08150582366447644</v>
+        <v>0.0815058236644764</v>
       </c>
       <c r="W8" t="n">
-        <v>0.02306022491483497</v>
+        <v>0.02306022491483527</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.07774297094939057</v>
+        <v>-0.07774297094939064</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.06837757927492243</v>
+        <v>0.06837757927492202</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.06111048046672687</v>
+        <v>0.06111048046672744</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.2779357062449813</v>
+        <v>-0.2779357062449828</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.0425276410490285</v>
+        <v>-0.04252764104902886</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1849532431283424</v>
+        <v>0.184953243128344</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.005426109759395126</v>
+        <v>0.005426109759395127</v>
       </c>
     </row>
     <row r="9">
@@ -1245,91 +1245,91 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.005327843942331428</v>
+        <v>0.005327843942332374</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.05595703662236306</v>
+        <v>-0.055957036622363</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1240683217221154</v>
+        <v>-0.1240683217221146</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1332431641180928</v>
+        <v>0.1332431641180914</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06749129753345921</v>
+        <v>0.06749129753345887</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01110522927200634</v>
+        <v>-0.01110522927200638</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1025703582654423</v>
+        <v>-0.1025703582654421</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.04955528768131071</v>
+        <v>-0.04955528768131019</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.05948150968660513</v>
+        <v>-0.05948150968660523</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.08493555240859298</v>
+        <v>-0.0849355524085927</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.04870524949385737</v>
+        <v>-0.04870524949385752</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01672970707055853</v>
+        <v>0.01672970707055827</v>
       </c>
       <c r="O9" t="n">
-        <v>0.03734049381615734</v>
+        <v>0.03734049381615713</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.1528584043154071</v>
+        <v>-0.1528584043154051</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.238684862569447</v>
+        <v>-0.2386848625694473</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1362566916341287</v>
+        <v>0.1362566916341276</v>
       </c>
       <c r="S9" t="n">
-        <v>0.04036997884390919</v>
+        <v>0.04036997884390901</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.09518456050552666</v>
+        <v>-0.09518456050552612</v>
       </c>
       <c r="U9" t="n">
-        <v>0.04955333063480254</v>
+        <v>0.04955333063480224</v>
       </c>
       <c r="V9" t="n">
-        <v>0.0391422141478881</v>
+        <v>0.03914221414788835</v>
       </c>
       <c r="W9" t="n">
-        <v>0.05948459823898915</v>
+        <v>0.05948459823898859</v>
       </c>
       <c r="X9" t="n">
-        <v>0.2163664193155169</v>
+        <v>0.216366419315517</v>
       </c>
       <c r="Y9" t="n">
-        <v>-0.001998790661104742</v>
+        <v>-0.001998790661104598</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.08980249677434596</v>
+        <v>-0.08980249677434621</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.01072743307583234</v>
+        <v>0.01072743307583241</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.1566592073495103</v>
+        <v>-0.1566592073495077</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.02058144507498651</v>
+        <v>-0.02058144507498658</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.007568510999958596</v>
+        <v>-0.007568510999958517</v>
       </c>
     </row>
     <row r="10">
@@ -1339,91 +1339,91 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.006751821148425145</v>
+        <v>-0.006751821148455144</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.06700792996032565</v>
+        <v>-0.06700792996032622</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2015400208497256</v>
+        <v>0.2015400208497262</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1588929993566444</v>
+        <v>-0.1588929993566437</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0867731770612358</v>
+        <v>0.08677317706123683</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09359933008622667</v>
+        <v>0.09359933008622548</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.08882547027173492</v>
+        <v>-0.08882547027173518</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.04955528768131071</v>
+        <v>-0.04955528768131019</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.3845128053578986</v>
+        <v>0.3845128053578956</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.01851781681925876</v>
+        <v>-0.01851781681925861</v>
       </c>
       <c r="M10" t="n">
-        <v>0.3670388156609222</v>
+        <v>0.3670388156609264</v>
       </c>
       <c r="N10" t="n">
-        <v>0.005383167161180205</v>
+        <v>0.005383167161179439</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.2719323436647439</v>
+        <v>-0.2719323436647421</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0903385784129466</v>
+        <v>0.09033857841294447</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0002792881348067672</v>
+        <v>-0.0002792881348068562</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.04049457658265238</v>
+        <v>-0.04049457658265254</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.191995806581865</v>
+        <v>-0.1919958065818623</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.05152459165661902</v>
+        <v>-0.05152459165661759</v>
       </c>
       <c r="U10" t="n">
-        <v>0.09624459835032548</v>
+        <v>0.09624459835032585</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.01492358163074341</v>
+        <v>-0.01492358163074491</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.1715391509211264</v>
+        <v>-0.171539150921126</v>
       </c>
       <c r="X10" t="n">
-        <v>0.004669191514805735</v>
+        <v>0.004669191514804882</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.04132731441204204</v>
+        <v>0.04132731441204129</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.418628273139917</v>
+        <v>0.4186282731399122</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.03807358625458487</v>
+        <v>0.03807358625458546</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.02671046812049771</v>
+        <v>-0.02671046812049832</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.02838062444699174</v>
+        <v>-0.02838062444699186</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.008696629340339374</v>
+        <v>-0.008696629340338642</v>
       </c>
     </row>
     <row r="11">
@@ -1433,91 +1433,91 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.004841507045589334</v>
+        <v>-0.004841507045589901</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.02412574075441339</v>
+        <v>-0.02412574075441358</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2244892493389906</v>
+        <v>0.2244892493389938</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1359016179997409</v>
+        <v>-0.1359016179997426</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.08367488681719192</v>
+        <v>-0.08367488681719261</v>
       </c>
       <c r="G11" t="n">
-        <v>0.04884581038940265</v>
+        <v>0.04884581038940244</v>
       </c>
       <c r="H11" t="n">
-        <v>0.03967748778025364</v>
+        <v>0.03967748778025409</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.05948150968660513</v>
+        <v>-0.05948150968660523</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3845128053578986</v>
+        <v>0.3845128053578956</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.05342650259919801</v>
+        <v>0.05342650259919828</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4110876095477534</v>
+        <v>0.4110876095477594</v>
       </c>
       <c r="N11" t="n">
-        <v>0.08191771164265173</v>
+        <v>0.08191771164265256</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.2023785527404742</v>
+        <v>-0.2023785527404748</v>
       </c>
       <c r="P11" t="n">
-        <v>0.1742900949981042</v>
+        <v>0.1742900949981046</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.01807801528670422</v>
+        <v>0.01807801528670424</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.0788989346277989</v>
+        <v>-0.07889893462779939</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.1685112394032636</v>
+        <v>-0.1685112394032638</v>
       </c>
       <c r="T11" t="n">
-        <v>0.03973043369083457</v>
+        <v>0.0397304336908347</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.06432922574812137</v>
+        <v>-0.06432922574812129</v>
       </c>
       <c r="V11" t="n">
-        <v>0.07419310337784719</v>
+        <v>0.0741931033778485</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.123419791418862</v>
+        <v>-0.1234197914188623</v>
       </c>
       <c r="X11" t="n">
-        <v>0.01160106055080736</v>
+        <v>0.0116010605508074</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.0843203672301677</v>
+        <v>0.08432036723016705</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.4193997560018921</v>
+        <v>0.419399756001895</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.01801223600408141</v>
+        <v>-0.01801223600408154</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.01440263580629541</v>
+        <v>0.01440263580629545</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.01724922605509062</v>
+        <v>-0.01724922605509092</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.004571282443345205</v>
+        <v>-0.004571282443345207</v>
       </c>
     </row>
     <row r="12">
@@ -1527,34 +1527,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.003810115400934034</v>
+        <v>-0.003810115400934361</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0567146391968809</v>
+        <v>0.05671463919688057</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1277295672132354</v>
+        <v>0.1277295672132343</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.09482163926037218</v>
+        <v>-0.09482163926037185</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.06399826795457438</v>
+        <v>-0.06399826795457476</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.06480089222744193</v>
+        <v>-0.06480089222744131</v>
       </c>
       <c r="H12" t="n">
-        <v>0.143380904978012</v>
+        <v>0.1433809049780099</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.08493555240859298</v>
+        <v>-0.0849355524085927</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.01851781681925876</v>
+        <v>-0.01851781681925861</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05342650259919801</v>
+        <v>0.05342650259919828</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -1563,55 +1563,55 @@
         <v>0.02047199712390744</v>
       </c>
       <c r="N12" t="n">
-        <v>0.04830854801234277</v>
+        <v>0.04830854801234268</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.04625105774419682</v>
+        <v>-0.04625105774419656</v>
       </c>
       <c r="P12" t="n">
-        <v>0.3389168996468365</v>
+        <v>0.3389168996468316</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.1592280812505132</v>
+        <v>0.1592280812505136</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.3242433743362566</v>
+        <v>-0.3242433743362535</v>
       </c>
       <c r="S12" t="n">
-        <v>0.02384017132183658</v>
+        <v>0.02384017132183637</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.06803133607450866</v>
+        <v>-0.06803133607450804</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.05220627135387299</v>
+        <v>-0.05220627135387255</v>
       </c>
       <c r="V12" t="n">
         <v>0.05862524183523415</v>
       </c>
       <c r="W12" t="n">
-        <v>0.03897303022562335</v>
+        <v>0.03897303022562301</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.07304035230077466</v>
+        <v>-0.07304035230077489</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.05257813613734297</v>
+        <v>0.05257813613734238</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.09762831260398891</v>
+        <v>0.09762831260398834</v>
       </c>
       <c r="AA12" t="n">
-        <v>-0.1584801244511936</v>
+        <v>-0.1584801244511909</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.04897913315473058</v>
+        <v>0.0489791331547308</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1466866568400333</v>
+        <v>0.1466866568400325</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.005873925907306308</v>
+        <v>0.005873925907306283</v>
       </c>
     </row>
     <row r="13">
@@ -1621,34 +1621,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.007806676320152247</v>
+        <v>-0.007806676320154338</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.02621911321679688</v>
+        <v>-0.02621911321679693</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2335739591475398</v>
+        <v>0.2335739591475378</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1841377598445468</v>
+        <v>-0.1841377598445477</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06695412066191682</v>
+        <v>0.066954120661917</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2183685993399871</v>
+        <v>0.2183685993399875</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01006404030103045</v>
+        <v>0.01006404030103051</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.04870524949385737</v>
+        <v>-0.04870524949385752</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3670388156609222</v>
+        <v>0.3670388156609264</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4110876095477534</v>
+        <v>0.4110876095477594</v>
       </c>
       <c r="L13" t="n">
         <v>0.02047199712390744</v>
@@ -1657,55 +1657,55 @@
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.04660949562149439</v>
+        <v>0.04660949562149531</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.1829286058876974</v>
+        <v>-0.182928605887696</v>
       </c>
       <c r="P13" t="n">
-        <v>0.1668272179865329</v>
+        <v>0.1668272179865334</v>
       </c>
       <c r="Q13" t="n">
         <v>-0.03234129421564733</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.03789591040141446</v>
+        <v>-0.0378959104014138</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.1734339124309823</v>
+        <v>-0.1734339124309821</v>
       </c>
       <c r="T13" t="n">
-        <v>0.09917256699637013</v>
+        <v>0.09917256699636898</v>
       </c>
       <c r="U13" t="n">
-        <v>0.07606573678238433</v>
+        <v>0.07606573678238399</v>
       </c>
       <c r="V13" t="n">
-        <v>0.03624412638198244</v>
+        <v>0.03624412638198272</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.1375542232090763</v>
+        <v>-0.1375542232090761</v>
       </c>
       <c r="X13" t="n">
-        <v>0.01943064813602745</v>
+        <v>0.0194306481360272</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.06490096721177659</v>
+        <v>0.06490096721177654</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.294661935766147</v>
+        <v>0.294661935766149</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.04040243838788274</v>
+        <v>0.04040243838788238</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.02113975537609375</v>
+        <v>0.02113975537609394</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.08553931658610614</v>
+        <v>-0.08553931658610728</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.01594584507032239</v>
+        <v>-0.01594584507032227</v>
       </c>
     </row>
     <row r="14">
@@ -1715,91 +1715,91 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001954009510615686</v>
+        <v>-0.00195400951064774</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02516347794757303</v>
+        <v>0.02516347794757306</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04104506306654939</v>
+        <v>0.04104506306654923</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01823123135068524</v>
+        <v>-0.01823123135068552</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0910335862665629</v>
+        <v>-0.09103358626656365</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0110671685484269</v>
+        <v>-0.01106716854842708</v>
       </c>
       <c r="H14" t="n">
-        <v>0.06650253986622809</v>
+        <v>0.0665025398662283</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01672970707055853</v>
+        <v>0.01672970707055827</v>
       </c>
       <c r="J14" t="n">
-        <v>0.005383167161180205</v>
+        <v>0.005383167161179439</v>
       </c>
       <c r="K14" t="n">
-        <v>0.08191771164265173</v>
+        <v>0.08191771164265256</v>
       </c>
       <c r="L14" t="n">
-        <v>0.04830854801234277</v>
+        <v>0.04830854801234268</v>
       </c>
       <c r="M14" t="n">
-        <v>0.04660949562149439</v>
+        <v>0.04660949562149531</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.02952856641754083</v>
+        <v>-0.02952856641754099</v>
       </c>
       <c r="P14" t="n">
-        <v>0.07559323031462437</v>
+        <v>0.07559323031462511</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.001959905721663105</v>
+        <v>-0.001959905721662655</v>
       </c>
       <c r="R14" t="n">
         <v>-0.02891601454621705</v>
       </c>
       <c r="S14" t="n">
-        <v>0.00413834562060411</v>
+        <v>0.004138345620604055</v>
       </c>
       <c r="T14" t="n">
-        <v>0.002471891210656967</v>
+        <v>0.002471891210657151</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.08360957169362936</v>
+        <v>-0.0836095716936293</v>
       </c>
       <c r="V14" t="n">
-        <v>0.2769890893549882</v>
+        <v>0.2769890893549912</v>
       </c>
       <c r="W14" t="n">
-        <v>0.005493622971748255</v>
+        <v>0.005493622971748145</v>
       </c>
       <c r="X14" t="n">
-        <v>0.02824352716558755</v>
+        <v>0.02824352716558699</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.3171485346167626</v>
+        <v>0.3171485346167659</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.03975230575459551</v>
+        <v>0.03975230575459618</v>
       </c>
       <c r="AA14" t="n">
-        <v>-0.03988356159728736</v>
+        <v>-0.03988356159728762</v>
       </c>
       <c r="AB14" t="n">
-        <v>-0.01023285931755932</v>
+        <v>-0.01023285931755931</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.01462849170605009</v>
+        <v>0.01462849170605047</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.00403940493930977</v>
+        <v>-0.004039404939309686</v>
       </c>
     </row>
     <row r="15">
@@ -1809,91 +1809,91 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.005819122517392793</v>
+        <v>0.005819122517400661</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.002006199593661507</v>
+        <v>-0.002006199593661595</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.1093791755856592</v>
+        <v>-0.1093791755856588</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06488022195694104</v>
+        <v>0.06488022195694118</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00817052050051075</v>
+        <v>0.00817052050051083</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.061446475280487</v>
+        <v>-0.06144647528048627</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.08329810050424556</v>
+        <v>-0.08329810050424651</v>
       </c>
       <c r="I15" t="n">
-        <v>0.03734049381615734</v>
+        <v>0.03734049381615713</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.2719323436647439</v>
+        <v>-0.2719323436647421</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.2023785527404742</v>
+        <v>-0.2023785527404748</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.04625105774419682</v>
+        <v>-0.04625105774419656</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.1829286058876974</v>
+        <v>-0.182928605887696</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.02952856641754083</v>
+        <v>-0.02952856641754099</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.066785040734088</v>
+        <v>-0.0667850407340876</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0471293049239919</v>
+        <v>-0.0471293049239921</v>
       </c>
       <c r="R15" t="n">
-        <v>0.07524189848482273</v>
+        <v>0.07524189848482225</v>
       </c>
       <c r="S15" t="n">
-        <v>0.06628040311839081</v>
+        <v>0.06628040311839152</v>
       </c>
       <c r="T15" t="n">
-        <v>0.02197973365535795</v>
+        <v>0.02197973365535772</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.01205772830388437</v>
+        <v>-0.0120577283038843</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.0500736734974245</v>
+        <v>-0.05007367349742452</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.001486675404982047</v>
+        <v>-0.001486675404982043</v>
       </c>
       <c r="X15" t="n">
-        <v>0.02387392725260604</v>
+        <v>0.02387392725260615</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.02634277216924662</v>
+        <v>-0.02634277216924639</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.273334554205385</v>
+        <v>-0.2733345542053844</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.05745802077997238</v>
+        <v>0.05745802077997256</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.0006378176445429979</v>
+        <v>0.0006378176445430287</v>
       </c>
       <c r="AC15" t="n">
-        <v>-0.04060749642768538</v>
+        <v>-0.04060749642768532</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.004234008957905523</v>
+        <v>-0.004234008957905654</v>
       </c>
     </row>
     <row r="16">
@@ -1903,91 +1903,91 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.008440869839978979</v>
+        <v>-0.008440869839974762</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04407645986771008</v>
+        <v>0.04407645986770938</v>
       </c>
       <c r="D16" t="n">
         <v>0.2134837274346892</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1610312267027513</v>
+        <v>-0.1610312267027528</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.06132815058585541</v>
+        <v>-0.0613281505858554</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05745204772809384</v>
+        <v>0.05745204772809313</v>
       </c>
       <c r="H16" t="n">
-        <v>0.08274365449228922</v>
+        <v>0.0827436544922879</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.1528584043154071</v>
+        <v>-0.1528584043154051</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0903385784129466</v>
+        <v>0.09033857841294447</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1742900949981042</v>
+        <v>0.1742900949981046</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3389168996468365</v>
+        <v>0.3389168996468316</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1668272179865329</v>
+        <v>0.1668272179865334</v>
       </c>
       <c r="N16" t="n">
-        <v>0.07559323031462437</v>
+        <v>0.07559323031462511</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.066785040734088</v>
+        <v>-0.0667850407340876</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1206655757628095</v>
+        <v>0.12066557576281</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.2661341157651934</v>
+        <v>-0.2661341157651884</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.0476528757368349</v>
+        <v>-0.04765287573683494</v>
       </c>
       <c r="T16" t="n">
-        <v>0.07423366367766554</v>
+        <v>0.07423366367766539</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.0546571183459256</v>
+        <v>-0.05465711834592464</v>
       </c>
       <c r="V16" t="n">
-        <v>0.04578199743103103</v>
+        <v>0.04578199743103059</v>
       </c>
       <c r="W16" t="n">
-        <v>0.002483263557514441</v>
+        <v>0.002483263557514474</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.05720384552394082</v>
+        <v>-0.05720384552393975</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.07505107035809171</v>
+        <v>0.07505107035809075</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.1967676808498794</v>
+        <v>0.1967676808498796</v>
       </c>
       <c r="AA16" t="n">
-        <v>-0.02532082955913859</v>
+        <v>-0.02532082955913861</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.1008427589567406</v>
+        <v>0.1008427589567409</v>
       </c>
       <c r="AC16" t="n">
-        <v>-0.005912817915373845</v>
+        <v>-0.005912817915373842</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.001272051356885095</v>
+        <v>0.001272051356885039</v>
       </c>
     </row>
     <row r="17">
@@ -1997,91 +1997,91 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01582495487227976</v>
+        <v>-0.0158249548722751</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1189735699689563</v>
+        <v>0.1189735699689564</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1232799394661991</v>
+        <v>0.1232799394662006</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.06471908231036244</v>
+        <v>-0.0647190823103629</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1424848395321638</v>
+        <v>-0.142484839532166</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.1017707294568489</v>
+        <v>-0.1017707294568498</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2116712719142572</v>
+        <v>0.2116712719142609</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.238684862569447</v>
+        <v>-0.2386848625694473</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.0002792881348067672</v>
+        <v>-0.0002792881348068562</v>
       </c>
       <c r="K17" t="n">
-        <v>0.01807801528670422</v>
+        <v>0.01807801528670424</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1592280812505132</v>
+        <v>0.1592280812505136</v>
       </c>
       <c r="M17" t="n">
         <v>-0.03234129421564733</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.001959905721663105</v>
+        <v>-0.001959905721662655</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.0471293049239919</v>
+        <v>-0.0471293049239921</v>
       </c>
       <c r="P17" t="n">
-        <v>0.1206655757628095</v>
+        <v>0.12066557576281</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.1885515900137784</v>
+        <v>-0.1885515900137815</v>
       </c>
       <c r="S17" t="n">
-        <v>0.04922211831063129</v>
+        <v>0.04922211831063145</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.1496110297052797</v>
+        <v>-0.1496110297052789</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.1036983427947809</v>
+        <v>-0.1036983427947815</v>
       </c>
       <c r="V17" t="n">
-        <v>0.001158733198858716</v>
+        <v>0.001158733198858404</v>
       </c>
       <c r="W17" t="n">
-        <v>0.03767108432824318</v>
+        <v>0.03767108432824352</v>
       </c>
       <c r="X17" t="n">
-        <v>-0.1315965272369776</v>
+        <v>-0.1315965272369781</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.001188264917783762</v>
+        <v>0.001188264917783321</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.09736058552480011</v>
+        <v>0.09736058552480042</v>
       </c>
       <c r="AA17" t="n">
-        <v>-0.1799348438948209</v>
+        <v>-0.1799348438948223</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.01928345916355012</v>
+        <v>0.01928345916355021</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.2774237764659986</v>
+        <v>0.2774237764659997</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.004219300638306309</v>
+        <v>0.004219300638306353</v>
       </c>
     </row>
     <row r="18">
@@ -2091,91 +2091,91 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002415649425692551</v>
+        <v>0.002415649425689274</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.04221801463848525</v>
+        <v>-0.04221801463848573</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.2211626770849093</v>
+        <v>-0.2211626770849112</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2137294667945424</v>
+        <v>0.2137294667945406</v>
       </c>
       <c r="F18" t="n">
-        <v>0.05363510207263694</v>
+        <v>0.05363510207263771</v>
       </c>
       <c r="G18" t="n">
-        <v>0.08547959274002555</v>
+        <v>0.08547959274002463</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.1602828742365812</v>
+        <v>-0.1602828742365819</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1362566916341287</v>
+        <v>0.1362566916341276</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.04049457658265238</v>
+        <v>-0.04049457658265254</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.0788989346277989</v>
+        <v>-0.07889893462779939</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.3242433743362566</v>
+        <v>-0.3242433743362535</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.03789591040141446</v>
+        <v>-0.0378959104014138</v>
       </c>
       <c r="N18" t="n">
         <v>-0.02891601454621705</v>
       </c>
       <c r="O18" t="n">
-        <v>0.07524189848482273</v>
+        <v>0.07524189848482225</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.2661341157651934</v>
+        <v>-0.2661341157651884</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.1885515900137784</v>
+        <v>-0.1885515900137815</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>0.02956655358049609</v>
+        <v>0.02956655358049646</v>
       </c>
       <c r="T18" t="n">
-        <v>0.1312233563446141</v>
+        <v>0.1312233563446148</v>
       </c>
       <c r="U18" t="n">
-        <v>0.03637625638365086</v>
+        <v>0.03637625638365068</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.04523204088140973</v>
+        <v>-0.0452320408814096</v>
       </c>
       <c r="W18" t="n">
-        <v>0.02985138372821246</v>
+        <v>0.02985138372821244</v>
       </c>
       <c r="X18" t="n">
-        <v>0.07424054917440127</v>
+        <v>0.07424054917440157</v>
       </c>
       <c r="Y18" t="n">
-        <v>-0.02442188641142184</v>
+        <v>-0.02442188641142185</v>
       </c>
       <c r="Z18" t="n">
-        <v>-0.1364583303218744</v>
+        <v>-0.1364583303218755</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1970722535658275</v>
+        <v>0.1970722535658289</v>
       </c>
       <c r="AB18" t="n">
-        <v>-0.01723209823915158</v>
+        <v>-0.01723209823915168</v>
       </c>
       <c r="AC18" t="n">
-        <v>-0.1640239568781167</v>
+        <v>-0.1640239568781177</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.004214917736628346</v>
+        <v>0.004214917736628417</v>
       </c>
     </row>
     <row r="19">
@@ -2185,91 +2185,91 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.0009807823932814451</v>
+        <v>-0.0009807823932810756</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0703432573653735</v>
+        <v>0.07034325736537461</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.1342813671830702</v>
+        <v>-0.1342813671830735</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2404141307388312</v>
+        <v>0.2404141307388295</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.1108649630770478</v>
+        <v>-0.1108649630770486</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.1396715866169304</v>
+        <v>-0.1396715866169305</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04686897793799374</v>
+        <v>0.04686897793799358</v>
       </c>
       <c r="I19" t="n">
-        <v>0.04036997884390919</v>
+        <v>0.04036997884390901</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.191995806581865</v>
+        <v>-0.1919958065818623</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.1685112394032636</v>
+        <v>-0.1685112394032638</v>
       </c>
       <c r="L19" t="n">
-        <v>0.02384017132183658</v>
+        <v>0.02384017132183637</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.1734339124309823</v>
+        <v>-0.1734339124309821</v>
       </c>
       <c r="N19" t="n">
-        <v>0.00413834562060411</v>
+        <v>0.004138345620604055</v>
       </c>
       <c r="O19" t="n">
-        <v>0.06628040311839081</v>
+        <v>0.06628040311839152</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.0476528757368349</v>
+        <v>-0.04765287573683494</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.04922211831063129</v>
+        <v>0.04922211831063145</v>
       </c>
       <c r="R19" t="n">
-        <v>0.02956655358049609</v>
+        <v>0.02956655358049646</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.1162433577448635</v>
+        <v>-0.116243357744863</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.1100962586465682</v>
+        <v>-0.1100962586465683</v>
       </c>
       <c r="V19" t="n">
-        <v>0.007222014700928612</v>
+        <v>0.007222014700928808</v>
       </c>
       <c r="W19" t="n">
-        <v>0.3806254518602838</v>
+        <v>0.3806254518602856</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.04302614111301006</v>
+        <v>-0.0430261411130105</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.03899381807571276</v>
+        <v>-0.03899381807571273</v>
       </c>
       <c r="Z19" t="n">
-        <v>-0.1907018238413989</v>
+        <v>-0.1907018238413995</v>
       </c>
       <c r="AA19" t="n">
-        <v>-0.07509590136447344</v>
+        <v>-0.07509590136447306</v>
       </c>
       <c r="AB19" t="n">
-        <v>-0.04155875220409568</v>
+        <v>-0.04155875220409529</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1281674556597133</v>
+        <v>0.1281674556597142</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.005855144767080836</v>
+        <v>0.005855144767080874</v>
       </c>
     </row>
     <row r="20">
@@ -2279,91 +2279,91 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003911157232878403</v>
+        <v>0.003911157232875786</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.003794108679387379</v>
+        <v>-0.003794108679387351</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03189711144304377</v>
+        <v>0.03189711144304385</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.08699327581894981</v>
+        <v>-0.08699327581894925</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.005657214339024754</v>
+        <v>-0.005657214339024872</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1474424934269196</v>
+        <v>0.1474424934269187</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.1027593134180955</v>
+        <v>-0.1027593134180966</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.09518456050552666</v>
+        <v>-0.09518456050552612</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.05152459165661902</v>
+        <v>-0.05152459165661759</v>
       </c>
       <c r="K20" t="n">
-        <v>0.03973043369083457</v>
+        <v>0.0397304336908347</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.06803133607450866</v>
+        <v>-0.06803133607450804</v>
       </c>
       <c r="M20" t="n">
-        <v>0.09917256699637013</v>
+        <v>0.09917256699636898</v>
       </c>
       <c r="N20" t="n">
-        <v>0.002471891210656967</v>
+        <v>0.002471891210657151</v>
       </c>
       <c r="O20" t="n">
-        <v>0.02197973365535795</v>
+        <v>0.02197973365535772</v>
       </c>
       <c r="P20" t="n">
-        <v>0.07423366367766554</v>
+        <v>0.07423366367766539</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.1496110297052797</v>
+        <v>-0.1496110297052789</v>
       </c>
       <c r="R20" t="n">
-        <v>0.1312233563446141</v>
+        <v>0.1312233563446148</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.1162433577448635</v>
+        <v>-0.116243357744863</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
       </c>
       <c r="U20" t="n">
-        <v>-0.006222482790362905</v>
+        <v>-0.006222482790362906</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.01596469403155534</v>
+        <v>-0.01596469403155529</v>
       </c>
       <c r="W20" t="n">
-        <v>-0.1145480770662147</v>
+        <v>-0.1145480770662144</v>
       </c>
       <c r="X20" t="n">
-        <v>0.04166142694064977</v>
+        <v>0.04166142694064947</v>
       </c>
       <c r="Y20" t="n">
-        <v>-0.00791022957328465</v>
+        <v>-0.007910229573284355</v>
       </c>
       <c r="Z20" t="n">
-        <v>-0.04008735733789861</v>
+        <v>-0.0400873573378986</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.2649765140623843</v>
+        <v>0.2649765140623823</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.399175587620446</v>
+        <v>0.3991755876204449</v>
       </c>
       <c r="AC20" t="n">
-        <v>-0.2752613552520646</v>
+        <v>-0.2752613552520687</v>
       </c>
       <c r="AD20" t="n">
-        <v>-0.0003191464164218972</v>
+        <v>-0.000319146416421815</v>
       </c>
     </row>
     <row r="21">
@@ -2373,91 +2373,91 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0005967040528228183</v>
+        <v>0.0005967040528196539</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.0457864802152591</v>
+        <v>-0.04578648021525925</v>
       </c>
       <c r="D21" t="n">
-        <v>0.05370476839399391</v>
+        <v>0.05370476839399382</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.1647399506653912</v>
+        <v>-0.1647399506653904</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5163389916032641</v>
+        <v>0.5163389916032668</v>
       </c>
       <c r="G21" t="n">
-        <v>0.376969338478802</v>
+        <v>0.3769693384788039</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.1563366399626703</v>
+        <v>-0.1563366399626698</v>
       </c>
       <c r="I21" t="n">
-        <v>0.04955333063480254</v>
+        <v>0.04955333063480224</v>
       </c>
       <c r="J21" t="n">
-        <v>0.09624459835032548</v>
+        <v>0.09624459835032585</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.06432922574812137</v>
+        <v>-0.06432922574812129</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.05220627135387299</v>
+        <v>-0.05220627135387255</v>
       </c>
       <c r="M21" t="n">
-        <v>0.07606573678238433</v>
+        <v>0.07606573678238399</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.08360957169362936</v>
+        <v>-0.0836095716936293</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.01205772830388437</v>
+        <v>-0.0120577283038843</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.0546571183459256</v>
+        <v>-0.05465711834592464</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.1036983427947809</v>
+        <v>-0.1036983427947815</v>
       </c>
       <c r="R21" t="n">
-        <v>0.03637625638365086</v>
+        <v>0.03637625638365068</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.1100962586465682</v>
+        <v>-0.1100962586465683</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.006222482790362905</v>
+        <v>-0.006222482790362906</v>
       </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
-        <v>-0.09490685529386887</v>
+        <v>-0.09490685529386866</v>
       </c>
       <c r="W21" t="n">
-        <v>-0.08993315044937226</v>
+        <v>-0.08993315044937188</v>
       </c>
       <c r="X21" t="n">
-        <v>0.05137300356690742</v>
+        <v>0.05137300356690737</v>
       </c>
       <c r="Y21" t="n">
-        <v>-0.04572244115179931</v>
+        <v>-0.0457224411517986</v>
       </c>
       <c r="Z21" t="n">
-        <v>-0.09735367517730913</v>
+        <v>-0.09735367517730961</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.1054395755929252</v>
+        <v>0.1054395755929258</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.01411537834941089</v>
+        <v>-0.01411537834941097</v>
       </c>
       <c r="AC21" t="n">
-        <v>-0.1191486611854633</v>
+        <v>-0.1191486611854626</v>
       </c>
       <c r="AD21" t="n">
-        <v>-0.01150736523704633</v>
+        <v>-0.01150736523704634</v>
       </c>
     </row>
     <row r="22">
@@ -2467,91 +2467,91 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.009497326623859647</v>
+        <v>0.009497326623880427</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02781125497952166</v>
+        <v>0.02781125497952147</v>
       </c>
       <c r="D22" t="n">
-        <v>0.03663948474760128</v>
+        <v>0.03663948474760147</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.009927045468401587</v>
+        <v>-0.009927045468401514</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.1089322791113128</v>
+        <v>-0.108932279111314</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.0317851142097036</v>
+        <v>-0.0317851142097037</v>
       </c>
       <c r="H22" t="n">
-        <v>0.08150582366447644</v>
+        <v>0.0815058236644764</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0391422141478881</v>
+        <v>0.03914221414788835</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.01492358163074341</v>
+        <v>-0.01492358163074491</v>
       </c>
       <c r="K22" t="n">
-        <v>0.07419310337784719</v>
+        <v>0.0741931033778485</v>
       </c>
       <c r="L22" t="n">
         <v>0.05862524183523415</v>
       </c>
       <c r="M22" t="n">
-        <v>0.03624412638198244</v>
+        <v>0.03624412638198272</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2769890893549882</v>
+        <v>0.2769890893549912</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.0500736734974245</v>
+        <v>-0.05007367349742452</v>
       </c>
       <c r="P22" t="n">
-        <v>0.04578199743103103</v>
+        <v>0.04578199743103059</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.001158733198858716</v>
+        <v>0.001158733198858404</v>
       </c>
       <c r="R22" t="n">
-        <v>-0.04523204088140973</v>
+        <v>-0.0452320408814096</v>
       </c>
       <c r="S22" t="n">
-        <v>0.007222014700928612</v>
+        <v>0.007222014700928808</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.01596469403155534</v>
+        <v>-0.01596469403155529</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.09490685529386887</v>
+        <v>-0.09490685529386866</v>
       </c>
       <c r="V22" t="n">
         <v>1</v>
       </c>
       <c r="W22" t="n">
-        <v>0.008672548460993218</v>
+        <v>0.008672548460993742</v>
       </c>
       <c r="X22" t="n">
         <v>0.02507139153947497</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.194847995901764</v>
+        <v>0.1948479959017654</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.06574572525098911</v>
+        <v>0.06574572525098915</v>
       </c>
       <c r="AA22" t="n">
-        <v>-0.06501755382351436</v>
+        <v>-0.06501755382351487</v>
       </c>
       <c r="AB22" t="n">
-        <v>-0.03042291402674981</v>
+        <v>-0.03042291402675012</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.03357945472238019</v>
+        <v>0.03357945472238014</v>
       </c>
       <c r="AD22" t="n">
-        <v>-0.01035051011862836</v>
+        <v>-0.01035051011862849</v>
       </c>
     </row>
     <row r="23">
@@ -2561,91 +2561,91 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.00294143258538511</v>
+        <v>0.002941432585387215</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04481943691241014</v>
+        <v>0.04481943691241003</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.1082499228745516</v>
+        <v>-0.1082499228745526</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1857402266390846</v>
+        <v>0.1857402266390854</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.09901520957340881</v>
+        <v>-0.09901520957341101</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.09664702363980367</v>
+        <v>-0.0966470236398032</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02306022491483497</v>
+        <v>0.02306022491483527</v>
       </c>
       <c r="I23" t="n">
-        <v>0.05948459823898915</v>
+        <v>0.05948459823898859</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.1715391509211264</v>
+        <v>-0.171539150921126</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.123419791418862</v>
+        <v>-0.1234197914188623</v>
       </c>
       <c r="L23" t="n">
-        <v>0.03897303022562335</v>
+        <v>0.03897303022562301</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.1375542232090763</v>
+        <v>-0.1375542232090761</v>
       </c>
       <c r="N23" t="n">
-        <v>0.005493622971748255</v>
+        <v>0.005493622971748145</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.001486675404982047</v>
+        <v>-0.001486675404982043</v>
       </c>
       <c r="P23" t="n">
-        <v>0.002483263557514441</v>
+        <v>0.002483263557514474</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.03767108432824318</v>
+        <v>0.03767108432824352</v>
       </c>
       <c r="R23" t="n">
-        <v>0.02985138372821246</v>
+        <v>0.02985138372821244</v>
       </c>
       <c r="S23" t="n">
-        <v>0.3806254518602838</v>
+        <v>0.3806254518602856</v>
       </c>
       <c r="T23" t="n">
-        <v>-0.1145480770662147</v>
+        <v>-0.1145480770662144</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.08993315044937226</v>
+        <v>-0.08993315044937188</v>
       </c>
       <c r="V23" t="n">
-        <v>0.008672548460993218</v>
+        <v>0.008672548460993742</v>
       </c>
       <c r="W23" t="n">
         <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>-0.03439743460397045</v>
+        <v>-0.03439743460397074</v>
       </c>
       <c r="Y23" t="n">
-        <v>-0.03992561052943582</v>
+        <v>-0.03992561052943558</v>
       </c>
       <c r="Z23" t="n">
         <v>-0.1239194396450401</v>
       </c>
       <c r="AA23" t="n">
-        <v>-0.06425196938889448</v>
+        <v>-0.06425196938889498</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.04177486228621325</v>
+        <v>-0.04177486228621322</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.113877807614507</v>
+        <v>0.1138778076145084</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.003535987999010713</v>
+        <v>-0.003535987999010724</v>
       </c>
     </row>
     <row r="24">
@@ -2655,91 +2655,91 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.005003910971446085</v>
+        <v>0.005003910971445515</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.03586052257429424</v>
+        <v>-0.03586052257429406</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.06455220261611073</v>
+        <v>-0.06455220261611086</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0104821308149696</v>
+        <v>0.01048213081496965</v>
       </c>
       <c r="F24" t="n">
-        <v>0.07358670042198172</v>
+        <v>0.07358670042198175</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0481119669913073</v>
+        <v>0.04811196699130717</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.07774297094939057</v>
+        <v>-0.07774297094939064</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2163664193155169</v>
+        <v>0.216366419315517</v>
       </c>
       <c r="J24" t="n">
-        <v>0.004669191514805735</v>
+        <v>0.004669191514804882</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01160106055080736</v>
+        <v>0.0116010605508074</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.07304035230077466</v>
+        <v>-0.07304035230077489</v>
       </c>
       <c r="M24" t="n">
-        <v>0.01943064813602745</v>
+        <v>0.0194306481360272</v>
       </c>
       <c r="N24" t="n">
-        <v>0.02824352716558755</v>
+        <v>0.02824352716558699</v>
       </c>
       <c r="O24" t="n">
-        <v>0.02387392725260604</v>
+        <v>0.02387392725260615</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.05720384552394082</v>
+        <v>-0.05720384552393975</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.1315965272369776</v>
+        <v>-0.1315965272369781</v>
       </c>
       <c r="R24" t="n">
-        <v>0.07424054917440127</v>
+        <v>0.07424054917440157</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.04302614111301006</v>
+        <v>-0.0430261411130105</v>
       </c>
       <c r="T24" t="n">
-        <v>0.04166142694064977</v>
+        <v>0.04166142694064947</v>
       </c>
       <c r="U24" t="n">
-        <v>0.05137300356690742</v>
+        <v>0.05137300356690737</v>
       </c>
       <c r="V24" t="n">
         <v>0.02507139153947497</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.03439743460397045</v>
+        <v>-0.03439743460397074</v>
       </c>
       <c r="X24" t="n">
         <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.01772476306817729</v>
+        <v>0.01772476306817717</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.03673256970492826</v>
+        <v>-0.03673256970492848</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.0959264520648508</v>
+        <v>0.09592645206485115</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.01631311760248449</v>
+        <v>-0.01631311760248442</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.1278918315237322</v>
+        <v>-0.1278918315237328</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.004864805940135796</v>
+        <v>-0.004864805940135792</v>
       </c>
     </row>
     <row r="25">
@@ -2749,91 +2749,91 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0008010430298134766</v>
+        <v>0.0008010430298419018</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01252001634972355</v>
+        <v>0.01252001634972327</v>
       </c>
       <c r="D25" t="n">
-        <v>0.08380594414087869</v>
+        <v>0.08380594414087833</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.06123995584416318</v>
+        <v>-0.06123995584416266</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.04788222386583824</v>
+        <v>-0.04788222386583884</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0168810522622406</v>
+        <v>0.01688105226224053</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06837757927492243</v>
+        <v>0.06837757927492202</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.001998790661104742</v>
+        <v>-0.001998790661104598</v>
       </c>
       <c r="J25" t="n">
-        <v>0.04132731441204204</v>
+        <v>0.04132731441204129</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0843203672301677</v>
+        <v>0.08432036723016705</v>
       </c>
       <c r="L25" t="n">
-        <v>0.05257813613734297</v>
+        <v>0.05257813613734238</v>
       </c>
       <c r="M25" t="n">
-        <v>0.06490096721177659</v>
+        <v>0.06490096721177654</v>
       </c>
       <c r="N25" t="n">
-        <v>0.3171485346167626</v>
+        <v>0.3171485346167659</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.02634277216924662</v>
+        <v>-0.02634277216924639</v>
       </c>
       <c r="P25" t="n">
-        <v>0.07505107035809171</v>
+        <v>0.07505107035809075</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.001188264917783762</v>
+        <v>0.001188264917783321</v>
       </c>
       <c r="R25" t="n">
-        <v>-0.02442188641142184</v>
+        <v>-0.02442188641142185</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.03899381807571276</v>
+        <v>-0.03899381807571273</v>
       </c>
       <c r="T25" t="n">
-        <v>-0.00791022957328465</v>
+        <v>-0.007910229573284355</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.04572244115179931</v>
+        <v>-0.0457224411517986</v>
       </c>
       <c r="V25" t="n">
-        <v>0.194847995901764</v>
+        <v>0.1948479959017654</v>
       </c>
       <c r="W25" t="n">
-        <v>-0.03992561052943582</v>
+        <v>-0.03992561052943558</v>
       </c>
       <c r="X25" t="n">
-        <v>0.01772476306817729</v>
+        <v>0.01772476306817717</v>
       </c>
       <c r="Y25" t="n">
         <v>1</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.05814250555685131</v>
+        <v>0.05814250555685081</v>
       </c>
       <c r="AA25" t="n">
-        <v>-0.03068827985653607</v>
+        <v>-0.03068827985653568</v>
       </c>
       <c r="AB25" t="n">
-        <v>-0.02580622794139138</v>
+        <v>-0.02580622794139104</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.00606336406933179</v>
+        <v>0.006063364069331443</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.01023912269725023</v>
+        <v>0.01023912269724998</v>
       </c>
     </row>
     <row r="26">
@@ -2843,91 +2843,91 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.009408097150011193</v>
+        <v>-0.009408097150033113</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.003483363700040023</v>
+        <v>-0.003483363700039383</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2568660344935301</v>
+        <v>0.25686603449353</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.1421976854004574</v>
+        <v>-0.142197685400458</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.1206321809120477</v>
+        <v>-0.1206321809120494</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.05101035330868514</v>
+        <v>-0.05101035330868505</v>
       </c>
       <c r="H26" t="n">
-        <v>0.06111048046672687</v>
+        <v>0.06111048046672744</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.08980249677434596</v>
+        <v>-0.08980249677434621</v>
       </c>
       <c r="J26" t="n">
-        <v>0.418628273139917</v>
+        <v>0.4186282731399122</v>
       </c>
       <c r="K26" t="n">
-        <v>0.4193997560018921</v>
+        <v>0.419399756001895</v>
       </c>
       <c r="L26" t="n">
-        <v>0.09762831260398891</v>
+        <v>0.09762831260398834</v>
       </c>
       <c r="M26" t="n">
-        <v>0.294661935766147</v>
+        <v>0.294661935766149</v>
       </c>
       <c r="N26" t="n">
-        <v>0.03975230575459551</v>
+        <v>0.03975230575459618</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.273334554205385</v>
+        <v>-0.2733345542053844</v>
       </c>
       <c r="P26" t="n">
-        <v>0.1967676808498794</v>
+        <v>0.1967676808498796</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.09736058552480011</v>
+        <v>0.09736058552480042</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.1364583303218744</v>
+        <v>-0.1364583303218755</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.1907018238413989</v>
+        <v>-0.1907018238413995</v>
       </c>
       <c r="T26" t="n">
-        <v>-0.04008735733789861</v>
+        <v>-0.0400873573378986</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.09735367517730913</v>
+        <v>-0.09735367517730961</v>
       </c>
       <c r="V26" t="n">
-        <v>0.06574572525098911</v>
+        <v>0.06574572525098915</v>
       </c>
       <c r="W26" t="n">
         <v>-0.1239194396450401</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.03673256970492826</v>
+        <v>-0.03673256970492848</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.05814250555685131</v>
+        <v>0.05814250555685081</v>
       </c>
       <c r="Z26" t="n">
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>-0.06669705207424759</v>
+        <v>-0.06669705207424814</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.006869661419212199</v>
+        <v>0.006869661419212299</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.06741003509163665</v>
+        <v>0.0674100350916374</v>
       </c>
       <c r="AD26" t="n">
-        <v>-0.001824929626409422</v>
+        <v>-0.001824929626409262</v>
       </c>
     </row>
     <row r="27">
@@ -2937,91 +2937,91 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.005426099532313172</v>
+        <v>0.005426099532319414</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.06612944381389659</v>
+        <v>-0.06612944381389728</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.02677572435974134</v>
+        <v>-0.02677572435974145</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.05087008587199935</v>
+        <v>-0.05087008587199974</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1230084554100948</v>
+        <v>0.123008455410096</v>
       </c>
       <c r="G27" t="n">
-        <v>0.09573980675138585</v>
+        <v>0.0957398067513857</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.2779357062449813</v>
+        <v>-0.2779357062449828</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01072743307583234</v>
+        <v>0.01072743307583241</v>
       </c>
       <c r="J27" t="n">
-        <v>0.03807358625458487</v>
+        <v>0.03807358625458546</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.01801223600408141</v>
+        <v>-0.01801223600408154</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.1584801244511936</v>
+        <v>-0.1584801244511909</v>
       </c>
       <c r="M27" t="n">
-        <v>0.04040243838788274</v>
+        <v>0.04040243838788238</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.03988356159728736</v>
+        <v>-0.03988356159728762</v>
       </c>
       <c r="O27" t="n">
-        <v>0.05745802077997238</v>
+        <v>0.05745802077997256</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.02532082955913859</v>
+        <v>-0.02532082955913861</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.1799348438948209</v>
+        <v>-0.1799348438948223</v>
       </c>
       <c r="R27" t="n">
-        <v>0.1970722535658275</v>
+        <v>0.1970722535658289</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.07509590136447344</v>
+        <v>-0.07509590136447306</v>
       </c>
       <c r="T27" t="n">
-        <v>0.2649765140623843</v>
+        <v>0.2649765140623823</v>
       </c>
       <c r="U27" t="n">
-        <v>0.1054395755929252</v>
+        <v>0.1054395755929258</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.06501755382351436</v>
+        <v>-0.06501755382351487</v>
       </c>
       <c r="W27" t="n">
-        <v>-0.06425196938889448</v>
+        <v>-0.06425196938889498</v>
       </c>
       <c r="X27" t="n">
-        <v>0.0959264520648508</v>
+        <v>0.09592645206485115</v>
       </c>
       <c r="Y27" t="n">
-        <v>-0.03068827985653607</v>
+        <v>-0.03068827985653568</v>
       </c>
       <c r="Z27" t="n">
-        <v>-0.06669705207424759</v>
+        <v>-0.06669705207424814</v>
       </c>
       <c r="AA27" t="n">
         <v>1</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.1236080503189705</v>
+        <v>0.1236080503189714</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.3039817849297362</v>
+        <v>-0.3039817849297357</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.007492864367658199</v>
+        <v>0.007492864367658236</v>
       </c>
     </row>
     <row r="28">
@@ -3031,91 +3031,91 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.004392818585115982</v>
+        <v>-0.004392818585108846</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01355440587483</v>
+        <v>0.01355440587483003</v>
       </c>
       <c r="D28" t="n">
-        <v>0.04137257711004026</v>
+        <v>0.04137257711004009</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.07113979528195999</v>
+        <v>-0.07113979528195946</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.03274846807870237</v>
+        <v>-0.03274846807870244</v>
       </c>
       <c r="G28" t="n">
         <v>0.01094301655153136</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.0425276410490285</v>
+        <v>-0.04252764104902886</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.1566592073495103</v>
+        <v>-0.1566592073495077</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.02671046812049771</v>
+        <v>-0.02671046812049832</v>
       </c>
       <c r="K28" t="n">
-        <v>0.01440263580629541</v>
+        <v>0.01440263580629545</v>
       </c>
       <c r="L28" t="n">
-        <v>0.04897913315473058</v>
+        <v>0.0489791331547308</v>
       </c>
       <c r="M28" t="n">
-        <v>0.02113975537609375</v>
+        <v>0.02113975537609394</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.01023285931755932</v>
+        <v>-0.01023285931755931</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0006378176445429979</v>
+        <v>0.0006378176445430287</v>
       </c>
       <c r="P28" t="n">
-        <v>0.1008427589567406</v>
+        <v>0.1008427589567409</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.01928345916355012</v>
+        <v>0.01928345916355021</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.01723209823915158</v>
+        <v>-0.01723209823915168</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.04155875220409568</v>
+        <v>-0.04155875220409529</v>
       </c>
       <c r="T28" t="n">
-        <v>0.399175587620446</v>
+        <v>0.3991755876204449</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.01411537834941089</v>
+        <v>-0.01411537834941097</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.03042291402674981</v>
+        <v>-0.03042291402675012</v>
       </c>
       <c r="W28" t="n">
-        <v>-0.04177486228621325</v>
+        <v>-0.04177486228621322</v>
       </c>
       <c r="X28" t="n">
-        <v>-0.01631311760248449</v>
+        <v>-0.01631311760248442</v>
       </c>
       <c r="Y28" t="n">
-        <v>-0.02580622794139138</v>
+        <v>-0.02580622794139104</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.006869661419212199</v>
+        <v>0.006869661419212299</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.1236080503189705</v>
+        <v>0.1236080503189714</v>
       </c>
       <c r="AB28" t="n">
         <v>1</v>
       </c>
       <c r="AC28" t="n">
-        <v>-0.09880866491964305</v>
+        <v>-0.09880866491964291</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.0087624220815885</v>
+        <v>-0.008762422081588559</v>
       </c>
     </row>
     <row r="29">
@@ -3125,91 +3125,91 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.01082710065890333</v>
+        <v>-0.01082710065890251</v>
       </c>
       <c r="C29" t="n">
-        <v>0.084200907631323</v>
+        <v>0.0842009076313236</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01170716638941757</v>
+        <v>0.01170716638941756</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0815357273759923</v>
+        <v>0.08153572737599282</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.1495979406489637</v>
+        <v>-0.1495979406489656</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.161372168774144</v>
+        <v>-0.1613721687741443</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1849532431283424</v>
+        <v>0.184953243128344</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02058144507498651</v>
+        <v>-0.02058144507498658</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.02838062444699174</v>
+        <v>-0.02838062444699186</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.01724922605509062</v>
+        <v>-0.01724922605509092</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1466866568400333</v>
+        <v>0.1466866568400325</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.08553931658610614</v>
+        <v>-0.08553931658610728</v>
       </c>
       <c r="N29" t="n">
-        <v>0.01462849170605009</v>
+        <v>0.01462849170605047</v>
       </c>
       <c r="O29" t="n">
-        <v>-0.04060749642768538</v>
+        <v>-0.04060749642768532</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.005912817915373845</v>
+        <v>-0.005912817915373842</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.2774237764659986</v>
+        <v>0.2774237764659997</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.1640239568781167</v>
+        <v>-0.1640239568781177</v>
       </c>
       <c r="S29" t="n">
-        <v>0.1281674556597133</v>
+        <v>0.1281674556597142</v>
       </c>
       <c r="T29" t="n">
-        <v>-0.2752613552520646</v>
+        <v>-0.2752613552520687</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.1191486611854633</v>
+        <v>-0.1191486611854626</v>
       </c>
       <c r="V29" t="n">
-        <v>0.03357945472238019</v>
+        <v>0.03357945472238014</v>
       </c>
       <c r="W29" t="n">
-        <v>0.113877807614507</v>
+        <v>0.1138778076145084</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.1278918315237322</v>
+        <v>-0.1278918315237328</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.00606336406933179</v>
+        <v>0.006063364069331443</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.06741003509163665</v>
+        <v>0.0674100350916374</v>
       </c>
       <c r="AA29" t="n">
-        <v>-0.3039817849297362</v>
+        <v>-0.3039817849297357</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.09880866491964305</v>
+        <v>-0.09880866491964291</v>
       </c>
       <c r="AC29" t="n">
         <v>1</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.01329528552794521</v>
+        <v>-0.01329528552794536</v>
       </c>
     </row>
     <row r="30">
@@ -3225,82 +3225,82 @@
         <v>0.0106089585031679</v>
       </c>
       <c r="D30" t="n">
-        <v>0.00454472374132441</v>
+        <v>0.004544723741324472</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.009027057405997772</v>
+        <v>-0.009027057405997746</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001918246918019185</v>
+        <v>0.001918246918019261</v>
       </c>
       <c r="G30" t="n">
-        <v>0.000421366663336117</v>
+        <v>0.0004213666633361352</v>
       </c>
       <c r="H30" t="n">
-        <v>0.005426109759395126</v>
+        <v>0.005426109759395127</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.007568510999958596</v>
+        <v>-0.007568510999958517</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.008696629340339374</v>
+        <v>-0.008696629340338642</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.004571282443345205</v>
+        <v>-0.004571282443345207</v>
       </c>
       <c r="L30" t="n">
-        <v>0.005873925907306308</v>
+        <v>0.005873925907306283</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.01594584507032239</v>
+        <v>-0.01594584507032227</v>
       </c>
       <c r="N30" t="n">
-        <v>-0.00403940493930977</v>
+        <v>-0.004039404939309686</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.004234008957905523</v>
+        <v>-0.004234008957905654</v>
       </c>
       <c r="P30" t="n">
-        <v>0.001272051356885095</v>
+        <v>0.001272051356885039</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.004219300638306309</v>
+        <v>0.004219300638306353</v>
       </c>
       <c r="R30" t="n">
-        <v>0.004214917736628346</v>
+        <v>0.004214917736628417</v>
       </c>
       <c r="S30" t="n">
-        <v>0.005855144767080836</v>
+        <v>0.005855144767080874</v>
       </c>
       <c r="T30" t="n">
-        <v>-0.0003191464164218972</v>
+        <v>-0.000319146416421815</v>
       </c>
       <c r="U30" t="n">
-        <v>-0.01150736523704633</v>
+        <v>-0.01150736523704634</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.01035051011862836</v>
+        <v>-0.01035051011862849</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.003535987999010713</v>
+        <v>-0.003535987999010724</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.004864805940135796</v>
+        <v>-0.004864805940135792</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.01023912269725023</v>
+        <v>0.01023912269724998</v>
       </c>
       <c r="Z30" t="n">
-        <v>-0.001824929626409422</v>
+        <v>-0.001824929626409262</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.007492864367658199</v>
+        <v>0.007492864367658236</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.0087624220815885</v>
+        <v>-0.008762422081588559</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.01329528552794521</v>
+        <v>-0.01329528552794536</v>
       </c>
       <c r="AD30" t="n">
         <v>1</v>

</xml_diff>